<commit_message>
Changing Module 1 numbers
</commit_message>
<xml_diff>
--- a/T1.xlsx
+++ b/T1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\misha\Desktop\Questions\MCQ ggenerator\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A342406A-FCAD-4A41-ADDF-3E52882AA50B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41586242-42B0-4FC9-AB76-AD506AD066CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{7A0B5B63-34D5-48C3-845D-CEB04A106E87}"/>
   </bookViews>
@@ -5350,11 +5350,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{90D3818D-47CE-41E6-8913-CED8EE4E3F8A}">
-  <sheetPr filterMode="1"/>
   <dimension ref="A1:AC389"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A142" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D183" sqref="D183"/>
+    <sheetView tabSelected="1" topLeftCell="N103" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="J1" sqref="A1:J1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="23.4" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -5476,7 +5475,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="2" spans="1:29" ht="23.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:29" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -5537,7 +5536,7 @@
       <c r="AB2" s="2"/>
       <c r="AC2" s="2"/>
     </row>
-    <row r="3" spans="1:29" ht="23.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:29" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="2">
         <v>2</v>
       </c>
@@ -5598,7 +5597,7 @@
       <c r="AB3" s="2"/>
       <c r="AC3" s="2"/>
     </row>
-    <row r="4" spans="1:29" ht="23.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:29" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="2">
         <v>3</v>
       </c>
@@ -5659,7 +5658,7 @@
       <c r="AB4" s="2"/>
       <c r="AC4" s="2"/>
     </row>
-    <row r="5" spans="1:29" ht="23.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:29" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="2">
         <v>4</v>
       </c>
@@ -5720,7 +5719,7 @@
       <c r="AB5" s="2"/>
       <c r="AC5" s="2"/>
     </row>
-    <row r="6" spans="1:29" ht="23.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:29" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="2">
         <v>5</v>
       </c>
@@ -5781,7 +5780,7 @@
       <c r="AB6" s="2"/>
       <c r="AC6" s="2"/>
     </row>
-    <row r="7" spans="1:29" ht="23.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:29" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="2">
         <v>6</v>
       </c>
@@ -5842,7 +5841,7 @@
       <c r="AB7" s="2"/>
       <c r="AC7" s="2"/>
     </row>
-    <row r="8" spans="1:29" ht="23.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:29" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="2">
         <v>7</v>
       </c>
@@ -5903,7 +5902,7 @@
       <c r="AB8" s="2"/>
       <c r="AC8" s="2"/>
     </row>
-    <row r="9" spans="1:29" ht="23.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:29" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="2">
         <v>8</v>
       </c>
@@ -5964,7 +5963,7 @@
       <c r="AB9" s="2"/>
       <c r="AC9" s="2"/>
     </row>
-    <row r="10" spans="1:29" ht="23.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:29" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="2">
         <v>9</v>
       </c>
@@ -6025,7 +6024,7 @@
       <c r="AB10" s="2"/>
       <c r="AC10" s="2"/>
     </row>
-    <row r="11" spans="1:29" ht="23.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:29" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="2">
         <v>10</v>
       </c>
@@ -6086,7 +6085,7 @@
       <c r="AB11" s="2"/>
       <c r="AC11" s="2"/>
     </row>
-    <row r="12" spans="1:29" ht="23.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:29" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="2">
         <v>11</v>
       </c>
@@ -6147,7 +6146,7 @@
       <c r="AB12" s="2"/>
       <c r="AC12" s="2"/>
     </row>
-    <row r="13" spans="1:29" ht="23.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:29" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="2">
         <v>12</v>
       </c>
@@ -6208,7 +6207,7 @@
       <c r="AB13" s="2"/>
       <c r="AC13" s="2"/>
     </row>
-    <row r="14" spans="1:29" s="6" customFormat="1" ht="73.8" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:29" s="6" customFormat="1" ht="73.8" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="2">
         <v>13</v>
       </c>
@@ -6269,7 +6268,7 @@
       <c r="AB14" s="4"/>
       <c r="AC14" s="4"/>
     </row>
-    <row r="15" spans="1:29" ht="23.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:29" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="2">
         <v>14</v>
       </c>
@@ -6330,7 +6329,7 @@
       <c r="AB15" s="2"/>
       <c r="AC15" s="2"/>
     </row>
-    <row r="16" spans="1:29" ht="23.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:29" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="2">
         <v>15</v>
       </c>
@@ -6391,7 +6390,7 @@
       <c r="AB16" s="2"/>
       <c r="AC16" s="2"/>
     </row>
-    <row r="17" spans="1:29" ht="23.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:29" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="2">
         <v>16</v>
       </c>
@@ -6452,7 +6451,7 @@
       <c r="AB17" s="2"/>
       <c r="AC17" s="2"/>
     </row>
-    <row r="18" spans="1:29" ht="23.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:29" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="2">
         <v>17</v>
       </c>
@@ -6513,7 +6512,7 @@
       <c r="AB18" s="2"/>
       <c r="AC18" s="2"/>
     </row>
-    <row r="19" spans="1:29" s="6" customFormat="1" ht="46.2" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:29" s="6" customFormat="1" ht="46.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="2">
         <v>18</v>
       </c>
@@ -6574,7 +6573,7 @@
       <c r="AB19" s="4"/>
       <c r="AC19" s="4"/>
     </row>
-    <row r="20" spans="1:29" ht="23.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:29" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="2">
         <v>19</v>
       </c>
@@ -6635,7 +6634,7 @@
       <c r="AB20" s="2"/>
       <c r="AC20" s="2"/>
     </row>
-    <row r="21" spans="1:29" s="6" customFormat="1" ht="70.2" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:29" s="6" customFormat="1" ht="70.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="2">
         <v>20</v>
       </c>
@@ -6696,7 +6695,7 @@
       <c r="AB21" s="4"/>
       <c r="AC21" s="4"/>
     </row>
-    <row r="22" spans="1:29" ht="23.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:29" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="2">
         <v>21</v>
       </c>
@@ -6757,7 +6756,7 @@
       <c r="AB22" s="2"/>
       <c r="AC22" s="2"/>
     </row>
-    <row r="23" spans="1:29" ht="23.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:29" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="2">
         <v>22</v>
       </c>
@@ -6818,7 +6817,7 @@
       <c r="AB23" s="2"/>
       <c r="AC23" s="2"/>
     </row>
-    <row r="24" spans="1:29" ht="23.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:29" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="2">
         <v>23</v>
       </c>
@@ -6879,7 +6878,7 @@
       <c r="AB24" s="2"/>
       <c r="AC24" s="2"/>
     </row>
-    <row r="25" spans="1:29" s="6" customFormat="1" ht="58.2" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:29" s="6" customFormat="1" ht="58.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="2">
         <v>24</v>
       </c>
@@ -6940,7 +6939,7 @@
       <c r="AB25" s="4"/>
       <c r="AC25" s="4"/>
     </row>
-    <row r="26" spans="1:29" ht="23.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:29" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" s="2">
         <v>25</v>
       </c>
@@ -7001,7 +7000,7 @@
       <c r="AB26" s="2"/>
       <c r="AC26" s="2"/>
     </row>
-    <row r="27" spans="1:29" ht="23.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:29" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" s="2">
         <v>26</v>
       </c>
@@ -7062,7 +7061,7 @@
       <c r="AB27" s="2"/>
       <c r="AC27" s="2"/>
     </row>
-    <row r="28" spans="1:29" ht="23.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:29" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A28" s="2">
         <v>27</v>
       </c>
@@ -7123,7 +7122,7 @@
       <c r="AB28" s="2"/>
       <c r="AC28" s="2"/>
     </row>
-    <row r="29" spans="1:29" ht="23.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:29" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A29" s="2">
         <v>28</v>
       </c>
@@ -7184,7 +7183,7 @@
       <c r="AB29" s="2"/>
       <c r="AC29" s="2"/>
     </row>
-    <row r="30" spans="1:29" ht="23.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:29" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A30" s="2">
         <v>29</v>
       </c>
@@ -7245,7 +7244,7 @@
       <c r="AB30" s="2"/>
       <c r="AC30" s="2"/>
     </row>
-    <row r="31" spans="1:29" ht="23.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:29" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A31" s="2">
         <v>30</v>
       </c>
@@ -7306,7 +7305,7 @@
       <c r="AB31" s="2"/>
       <c r="AC31" s="2"/>
     </row>
-    <row r="32" spans="1:29" ht="23.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:29" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A32" s="2">
         <v>31</v>
       </c>
@@ -7367,7 +7366,7 @@
       <c r="AB32" s="2"/>
       <c r="AC32" s="2"/>
     </row>
-    <row r="33" spans="1:29" ht="23.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:29" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A33" s="2">
         <v>32</v>
       </c>
@@ -7428,7 +7427,7 @@
       <c r="AB33" s="2"/>
       <c r="AC33" s="2"/>
     </row>
-    <row r="34" spans="1:29" ht="23.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:29" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A34" s="2">
         <v>33</v>
       </c>
@@ -7489,7 +7488,7 @@
       <c r="AB34" s="2"/>
       <c r="AC34" s="2"/>
     </row>
-    <row r="35" spans="1:29" ht="23.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:29" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A35" s="2">
         <v>34</v>
       </c>
@@ -7550,7 +7549,7 @@
       <c r="AB35" s="2"/>
       <c r="AC35" s="2"/>
     </row>
-    <row r="36" spans="1:29" ht="23.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:29" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A36" s="2">
         <v>35</v>
       </c>
@@ -7594,7 +7593,7 @@
       <c r="O36" s="2"/>
       <c r="P36" s="2"/>
       <c r="Q36" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="R36" s="2" t="s">
         <v>31</v>
@@ -7611,7 +7610,7 @@
       <c r="AB36" s="2"/>
       <c r="AC36" s="2"/>
     </row>
-    <row r="37" spans="1:29" ht="23.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:29" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A37" s="2">
         <v>36</v>
       </c>
@@ -7655,7 +7654,7 @@
       <c r="O37" s="2"/>
       <c r="P37" s="2"/>
       <c r="Q37" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="R37" s="2" t="s">
         <v>28</v>
@@ -7672,7 +7671,7 @@
       <c r="AB37" s="2"/>
       <c r="AC37" s="2"/>
     </row>
-    <row r="38" spans="1:29" ht="23.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:29" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A38" s="2">
         <v>37</v>
       </c>
@@ -7716,7 +7715,7 @@
       <c r="O38" s="2"/>
       <c r="P38" s="2"/>
       <c r="Q38" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="R38" s="2" t="s">
         <v>31</v>
@@ -7733,7 +7732,7 @@
       <c r="AB38" s="2"/>
       <c r="AC38" s="2"/>
     </row>
-    <row r="39" spans="1:29" ht="23.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:29" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A39" s="2">
         <v>38</v>
       </c>
@@ -7777,7 +7776,7 @@
       <c r="O39" s="2"/>
       <c r="P39" s="2"/>
       <c r="Q39" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="R39" s="2" t="s">
         <v>28</v>
@@ -7794,7 +7793,7 @@
       <c r="AB39" s="2"/>
       <c r="AC39" s="2"/>
     </row>
-    <row r="40" spans="1:29" ht="23.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:29" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A40" s="2">
         <v>39</v>
       </c>
@@ -7838,7 +7837,7 @@
       <c r="O40" s="2"/>
       <c r="P40" s="2"/>
       <c r="Q40" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="R40" s="2" t="s">
         <v>31</v>
@@ -7855,7 +7854,7 @@
       <c r="AB40" s="2"/>
       <c r="AC40" s="2"/>
     </row>
-    <row r="41" spans="1:29" ht="23.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:29" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A41" s="2">
         <v>40</v>
       </c>
@@ -7899,7 +7898,7 @@
       <c r="O41" s="2"/>
       <c r="P41" s="2"/>
       <c r="Q41" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="R41" s="2" t="s">
         <v>31</v>
@@ -7916,7 +7915,7 @@
       <c r="AB41" s="2"/>
       <c r="AC41" s="2"/>
     </row>
-    <row r="42" spans="1:29" ht="23.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:29" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A42" s="2">
         <v>41</v>
       </c>
@@ -7960,7 +7959,7 @@
       <c r="O42" s="2"/>
       <c r="P42" s="2"/>
       <c r="Q42" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="R42" s="2" t="s">
         <v>31</v>
@@ -7977,7 +7976,7 @@
       <c r="AB42" s="2"/>
       <c r="AC42" s="2"/>
     </row>
-    <row r="43" spans="1:29" ht="23.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:29" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A43" s="2">
         <v>42</v>
       </c>
@@ -8021,7 +8020,7 @@
       <c r="O43" s="2"/>
       <c r="P43" s="2"/>
       <c r="Q43" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="R43" s="2" t="s">
         <v>31</v>
@@ -8038,7 +8037,7 @@
       <c r="AB43" s="2"/>
       <c r="AC43" s="2"/>
     </row>
-    <row r="44" spans="1:29" ht="23.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:29" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A44" s="2">
         <v>43</v>
       </c>
@@ -8082,7 +8081,7 @@
       <c r="O44" s="2"/>
       <c r="P44" s="2"/>
       <c r="Q44" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="R44" s="2" t="s">
         <v>31</v>
@@ -8099,7 +8098,7 @@
       <c r="AB44" s="2"/>
       <c r="AC44" s="2"/>
     </row>
-    <row r="45" spans="1:29" ht="23.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:29" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A45" s="2">
         <v>44</v>
       </c>
@@ -8143,7 +8142,7 @@
       <c r="O45" s="2"/>
       <c r="P45" s="2"/>
       <c r="Q45" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="R45" s="2" t="s">
         <v>31</v>
@@ -8160,7 +8159,7 @@
       <c r="AB45" s="2"/>
       <c r="AC45" s="2"/>
     </row>
-    <row r="46" spans="1:29" ht="23.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:29" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A46" s="2">
         <v>45</v>
       </c>
@@ -8204,7 +8203,7 @@
       <c r="O46" s="2"/>
       <c r="P46" s="2"/>
       <c r="Q46" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="R46" s="2" t="s">
         <v>31</v>
@@ -8221,7 +8220,7 @@
       <c r="AB46" s="2"/>
       <c r="AC46" s="2"/>
     </row>
-    <row r="47" spans="1:29" ht="23.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:29" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A47" s="2">
         <v>46</v>
       </c>
@@ -8265,7 +8264,7 @@
       <c r="O47" s="2"/>
       <c r="P47" s="2"/>
       <c r="Q47" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="R47" s="2" t="s">
         <v>28</v>
@@ -8282,7 +8281,7 @@
       <c r="AB47" s="2"/>
       <c r="AC47" s="2"/>
     </row>
-    <row r="48" spans="1:29" ht="23.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:29" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A48" s="2">
         <v>47</v>
       </c>
@@ -8326,7 +8325,7 @@
       <c r="O48" s="2"/>
       <c r="P48" s="2"/>
       <c r="Q48" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="R48" s="2" t="s">
         <v>31</v>
@@ -8343,7 +8342,7 @@
       <c r="AB48" s="2"/>
       <c r="AC48" s="2"/>
     </row>
-    <row r="49" spans="1:29" ht="23.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:29" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A49" s="2">
         <v>48</v>
       </c>
@@ -8387,7 +8386,7 @@
       <c r="O49" s="2"/>
       <c r="P49" s="2"/>
       <c r="Q49" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="R49" s="2" t="s">
         <v>31</v>
@@ -8404,7 +8403,7 @@
       <c r="AB49" s="2"/>
       <c r="AC49" s="2"/>
     </row>
-    <row r="50" spans="1:29" ht="23.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:29" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A50" s="2">
         <v>49</v>
       </c>
@@ -8448,7 +8447,7 @@
       <c r="O50" s="2"/>
       <c r="P50" s="2"/>
       <c r="Q50" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="R50" s="2" t="s">
         <v>31</v>
@@ -8465,7 +8464,7 @@
       <c r="AB50" s="2"/>
       <c r="AC50" s="2"/>
     </row>
-    <row r="51" spans="1:29" ht="23.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:29" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A51" s="2">
         <v>50</v>
       </c>
@@ -8509,7 +8508,7 @@
       <c r="O51" s="2"/>
       <c r="P51" s="2"/>
       <c r="Q51" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="R51" s="2" t="s">
         <v>31</v>
@@ -8526,7 +8525,7 @@
       <c r="AB51" s="2"/>
       <c r="AC51" s="2"/>
     </row>
-    <row r="52" spans="1:29" ht="23.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:29" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A52" s="2">
         <v>51</v>
       </c>
@@ -8570,7 +8569,7 @@
       <c r="O52" s="2"/>
       <c r="P52" s="2"/>
       <c r="Q52" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="R52" s="2" t="s">
         <v>31</v>
@@ -8587,7 +8586,7 @@
       <c r="AB52" s="2"/>
       <c r="AC52" s="2"/>
     </row>
-    <row r="53" spans="1:29" ht="23.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:29" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A53" s="2">
         <v>52</v>
       </c>
@@ -8631,7 +8630,7 @@
       <c r="O53" s="2"/>
       <c r="P53" s="2"/>
       <c r="Q53" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="R53" s="2" t="s">
         <v>31</v>
@@ -8648,7 +8647,7 @@
       <c r="AB53" s="2"/>
       <c r="AC53" s="2"/>
     </row>
-    <row r="54" spans="1:29" ht="23.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:29" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A54" s="2">
         <v>53</v>
       </c>
@@ -8692,7 +8691,7 @@
       <c r="O54" s="2"/>
       <c r="P54" s="2"/>
       <c r="Q54" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="R54" s="2" t="s">
         <v>31</v>
@@ -8709,7 +8708,7 @@
       <c r="AB54" s="2"/>
       <c r="AC54" s="2"/>
     </row>
-    <row r="55" spans="1:29" ht="23.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:29" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A55" s="2">
         <v>54</v>
       </c>
@@ -8753,7 +8752,7 @@
       <c r="O55" s="2"/>
       <c r="P55" s="2"/>
       <c r="Q55" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="R55" s="2" t="s">
         <v>31</v>
@@ -8770,7 +8769,7 @@
       <c r="AB55" s="2"/>
       <c r="AC55" s="2"/>
     </row>
-    <row r="56" spans="1:29" ht="23.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:29" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A56" s="2">
         <v>55</v>
       </c>
@@ -8814,7 +8813,7 @@
       <c r="O56" s="2"/>
       <c r="P56" s="2"/>
       <c r="Q56" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="R56" s="2" t="s">
         <v>28</v>
@@ -8831,7 +8830,7 @@
       <c r="AB56" s="2"/>
       <c r="AC56" s="2"/>
     </row>
-    <row r="57" spans="1:29" ht="23.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:29" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A57" s="2">
         <v>56</v>
       </c>
@@ -8875,7 +8874,7 @@
       <c r="O57" s="2"/>
       <c r="P57" s="2"/>
       <c r="Q57" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="R57" s="2" t="s">
         <v>31</v>
@@ -8892,7 +8891,7 @@
       <c r="AB57" s="2"/>
       <c r="AC57" s="2"/>
     </row>
-    <row r="58" spans="1:29" ht="23.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:29" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A58" s="2">
         <v>57</v>
       </c>
@@ -8936,7 +8935,7 @@
       <c r="O58" s="2"/>
       <c r="P58" s="2"/>
       <c r="Q58" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="R58" s="2" t="s">
         <v>28</v>
@@ -8953,7 +8952,7 @@
       <c r="AB58" s="2"/>
       <c r="AC58" s="2"/>
     </row>
-    <row r="59" spans="1:29" ht="23.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:29" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A59" s="2">
         <v>58</v>
       </c>
@@ -8997,7 +8996,7 @@
       <c r="O59" s="2"/>
       <c r="P59" s="2"/>
       <c r="Q59" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="R59" s="2" t="s">
         <v>28</v>
@@ -9014,7 +9013,7 @@
       <c r="AB59" s="2"/>
       <c r="AC59" s="2"/>
     </row>
-    <row r="60" spans="1:29" ht="23.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:29" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A60" s="2">
         <v>59</v>
       </c>
@@ -9058,7 +9057,7 @@
       <c r="O60" s="2"/>
       <c r="P60" s="2"/>
       <c r="Q60" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="R60" s="2" t="s">
         <v>31</v>
@@ -9075,7 +9074,7 @@
       <c r="AB60" s="2"/>
       <c r="AC60" s="2"/>
     </row>
-    <row r="61" spans="1:29" ht="23.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:29" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A61" s="2">
         <v>60</v>
       </c>
@@ -9119,7 +9118,7 @@
       <c r="O61" s="2"/>
       <c r="P61" s="2"/>
       <c r="Q61" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="R61" s="2" t="s">
         <v>31</v>
@@ -9136,7 +9135,7 @@
       <c r="AB61" s="2"/>
       <c r="AC61" s="2"/>
     </row>
-    <row r="62" spans="1:29" ht="23.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:29" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A62" s="2">
         <v>61</v>
       </c>
@@ -9180,7 +9179,7 @@
       <c r="O62" s="2"/>
       <c r="P62" s="2"/>
       <c r="Q62" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="R62" s="2" t="s">
         <v>28</v>
@@ -9197,7 +9196,7 @@
       <c r="AB62" s="2"/>
       <c r="AC62" s="2"/>
     </row>
-    <row r="63" spans="1:29" ht="23.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:29" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A63" s="2">
         <v>62</v>
       </c>
@@ -9241,7 +9240,7 @@
       <c r="O63" s="2"/>
       <c r="P63" s="2"/>
       <c r="Q63" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="R63" s="2" t="s">
         <v>31</v>
@@ -9258,7 +9257,7 @@
       <c r="AB63" s="2"/>
       <c r="AC63" s="2"/>
     </row>
-    <row r="64" spans="1:29" ht="23.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:29" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A64" s="2">
         <v>63</v>
       </c>
@@ -9302,7 +9301,7 @@
       <c r="O64" s="2"/>
       <c r="P64" s="2"/>
       <c r="Q64" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="R64" s="2" t="s">
         <v>31</v>
@@ -9319,7 +9318,7 @@
       <c r="AB64" s="2"/>
       <c r="AC64" s="2"/>
     </row>
-    <row r="65" spans="1:29" ht="23.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:29" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A65" s="2">
         <v>64</v>
       </c>
@@ -9363,7 +9362,7 @@
       <c r="O65" s="2"/>
       <c r="P65" s="2"/>
       <c r="Q65" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="R65" s="2" t="s">
         <v>31</v>
@@ -9380,7 +9379,7 @@
       <c r="AB65" s="2"/>
       <c r="AC65" s="2"/>
     </row>
-    <row r="66" spans="1:29" ht="23.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:29" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A66" s="2">
         <v>65</v>
       </c>
@@ -9424,7 +9423,7 @@
       <c r="O66" s="2"/>
       <c r="P66" s="2"/>
       <c r="Q66" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="R66" s="2" t="s">
         <v>31</v>
@@ -9441,7 +9440,7 @@
       <c r="AB66" s="2"/>
       <c r="AC66" s="2"/>
     </row>
-    <row r="67" spans="1:29" ht="23.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:29" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A67" s="2">
         <v>66</v>
       </c>
@@ -9485,7 +9484,7 @@
       <c r="O67" s="2"/>
       <c r="P67" s="2"/>
       <c r="Q67" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="R67" s="2" t="s">
         <v>31</v>
@@ -9502,7 +9501,7 @@
       <c r="AB67" s="2"/>
       <c r="AC67" s="2"/>
     </row>
-    <row r="68" spans="1:29" ht="23.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:29" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A68" s="2">
         <v>67</v>
       </c>
@@ -9546,7 +9545,7 @@
       <c r="O68" s="2"/>
       <c r="P68" s="2"/>
       <c r="Q68" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="R68" s="2" t="s">
         <v>31</v>
@@ -9563,7 +9562,7 @@
       <c r="AB68" s="2"/>
       <c r="AC68" s="2"/>
     </row>
-    <row r="69" spans="1:29" ht="23.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:29" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A69" s="2">
         <v>68</v>
       </c>
@@ -9607,7 +9606,7 @@
       <c r="O69" s="2"/>
       <c r="P69" s="2"/>
       <c r="Q69" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="R69" s="2" t="s">
         <v>31</v>
@@ -9624,7 +9623,7 @@
       <c r="AB69" s="2"/>
       <c r="AC69" s="2"/>
     </row>
-    <row r="70" spans="1:29" ht="23.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:29" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A70" s="2">
         <v>69</v>
       </c>
@@ -9668,7 +9667,7 @@
       <c r="O70" s="2"/>
       <c r="P70" s="2"/>
       <c r="Q70" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="R70" s="2" t="s">
         <v>31</v>
@@ -9685,7 +9684,7 @@
       <c r="AB70" s="2"/>
       <c r="AC70" s="2"/>
     </row>
-    <row r="71" spans="1:29" ht="23.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:29" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A71" s="2">
         <v>70</v>
       </c>
@@ -9729,7 +9728,7 @@
       <c r="O71" s="2"/>
       <c r="P71" s="2"/>
       <c r="Q71" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="R71" s="2" t="s">
         <v>31</v>
@@ -9746,7 +9745,7 @@
       <c r="AB71" s="2"/>
       <c r="AC71" s="2"/>
     </row>
-    <row r="72" spans="1:29" ht="23.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:29" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A72" s="2">
         <v>71</v>
       </c>
@@ -9790,7 +9789,7 @@
       <c r="O72" s="2"/>
       <c r="P72" s="2"/>
       <c r="Q72" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="R72" s="2" t="s">
         <v>31</v>
@@ -9807,7 +9806,7 @@
       <c r="AB72" s="2"/>
       <c r="AC72" s="2"/>
     </row>
-    <row r="73" spans="1:29" ht="23.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:29" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A73" s="2">
         <v>72</v>
       </c>
@@ -9851,7 +9850,7 @@
       <c r="O73" s="2"/>
       <c r="P73" s="2"/>
       <c r="Q73" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="R73" s="2" t="s">
         <v>28</v>
@@ -9868,7 +9867,7 @@
       <c r="AB73" s="2"/>
       <c r="AC73" s="2"/>
     </row>
-    <row r="74" spans="1:29" ht="23.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:29" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A74" s="2">
         <v>73</v>
       </c>
@@ -9912,7 +9911,7 @@
       <c r="O74" s="2"/>
       <c r="P74" s="2"/>
       <c r="Q74" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="R74" s="2" t="s">
         <v>28</v>
@@ -9929,7 +9928,7 @@
       <c r="AB74" s="2"/>
       <c r="AC74" s="2"/>
     </row>
-    <row r="75" spans="1:29" ht="23.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:29" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A75" s="2">
         <v>74</v>
       </c>
@@ -9973,7 +9972,7 @@
       <c r="O75" s="2"/>
       <c r="P75" s="2"/>
       <c r="Q75" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="R75" s="2" t="s">
         <v>31</v>
@@ -9990,7 +9989,7 @@
       <c r="AB75" s="2"/>
       <c r="AC75" s="2"/>
     </row>
-    <row r="76" spans="1:29" ht="23.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:29" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A76" s="2">
         <v>75</v>
       </c>
@@ -10034,7 +10033,7 @@
       <c r="O76" s="2"/>
       <c r="P76" s="2"/>
       <c r="Q76" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="R76" s="2" t="s">
         <v>31</v>
@@ -10051,7 +10050,7 @@
       <c r="AB76" s="2"/>
       <c r="AC76" s="2"/>
     </row>
-    <row r="77" spans="1:29" ht="23.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:29" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A77" s="2">
         <v>76</v>
       </c>
@@ -10095,7 +10094,7 @@
       <c r="O77" s="2"/>
       <c r="P77" s="2"/>
       <c r="Q77" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="R77" s="8" t="s">
         <v>31</v>
@@ -10112,7 +10111,7 @@
       <c r="AB77" s="2"/>
       <c r="AC77" s="2"/>
     </row>
-    <row r="78" spans="1:29" ht="23.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:29" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A78" s="2">
         <v>77</v>
       </c>
@@ -10156,7 +10155,7 @@
       <c r="O78" s="2"/>
       <c r="P78" s="2"/>
       <c r="Q78" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="R78" s="2" t="s">
         <v>31</v>
@@ -10173,7 +10172,7 @@
       <c r="AB78" s="2"/>
       <c r="AC78" s="2"/>
     </row>
-    <row r="79" spans="1:29" ht="23.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:29" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A79" s="2">
         <v>78</v>
       </c>
@@ -10217,7 +10216,7 @@
       <c r="O79" s="2"/>
       <c r="P79" s="2"/>
       <c r="Q79" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="R79" s="2" t="s">
         <v>31</v>
@@ -10234,7 +10233,7 @@
       <c r="AB79" s="2"/>
       <c r="AC79" s="2"/>
     </row>
-    <row r="80" spans="1:29" ht="23.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:29" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A80" s="2">
         <v>79</v>
       </c>
@@ -10278,7 +10277,7 @@
       <c r="O80" s="2"/>
       <c r="P80" s="2"/>
       <c r="Q80" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="R80" s="2" t="s">
         <v>31</v>
@@ -10295,7 +10294,7 @@
       <c r="AB80" s="2"/>
       <c r="AC80" s="2"/>
     </row>
-    <row r="81" spans="1:29" ht="23.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:29" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A81" s="2">
         <v>80</v>
       </c>
@@ -10339,7 +10338,7 @@
       <c r="O81" s="2"/>
       <c r="P81" s="2"/>
       <c r="Q81" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="R81" s="2" t="s">
         <v>31</v>
@@ -10356,7 +10355,7 @@
       <c r="AB81" s="2"/>
       <c r="AC81" s="2"/>
     </row>
-    <row r="82" spans="1:29" ht="23.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:29" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A82" s="2">
         <v>81</v>
       </c>
@@ -10400,7 +10399,7 @@
       <c r="O82" s="2"/>
       <c r="P82" s="2"/>
       <c r="Q82" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="R82" s="2" t="s">
         <v>31</v>
@@ -10417,7 +10416,7 @@
       <c r="AB82" s="2"/>
       <c r="AC82" s="2"/>
     </row>
-    <row r="83" spans="1:29" ht="23.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:29" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A83" s="2">
         <v>82</v>
       </c>
@@ -10461,7 +10460,7 @@
       <c r="O83" s="2"/>
       <c r="P83" s="2"/>
       <c r="Q83" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="R83" s="2" t="s">
         <v>31</v>
@@ -10478,7 +10477,7 @@
       <c r="AB83" s="2"/>
       <c r="AC83" s="2"/>
     </row>
-    <row r="84" spans="1:29" ht="23.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:29" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A84" s="2">
         <v>83</v>
       </c>
@@ -10522,7 +10521,7 @@
       <c r="O84" s="2"/>
       <c r="P84" s="2"/>
       <c r="Q84" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="R84" s="2" t="s">
         <v>31</v>
@@ -10539,7 +10538,7 @@
       <c r="AB84" s="2"/>
       <c r="AC84" s="2"/>
     </row>
-    <row r="85" spans="1:29" ht="23.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:29" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A85" s="2">
         <v>84</v>
       </c>
@@ -10583,7 +10582,7 @@
       <c r="O85" s="2"/>
       <c r="P85" s="2"/>
       <c r="Q85" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="R85" s="2" t="s">
         <v>31</v>
@@ -10600,7 +10599,7 @@
       <c r="AB85" s="2"/>
       <c r="AC85" s="2"/>
     </row>
-    <row r="86" spans="1:29" ht="23.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:29" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A86" s="2">
         <v>85</v>
       </c>
@@ -10644,7 +10643,7 @@
       <c r="O86" s="2"/>
       <c r="P86" s="2"/>
       <c r="Q86" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="R86" s="2" t="s">
         <v>31</v>
@@ -10661,7 +10660,7 @@
       <c r="AB86" s="2"/>
       <c r="AC86" s="2"/>
     </row>
-    <row r="87" spans="1:29" ht="23.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:29" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A87" s="2">
         <v>86</v>
       </c>
@@ -10705,7 +10704,7 @@
       <c r="O87" s="2"/>
       <c r="P87" s="2"/>
       <c r="Q87" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="R87" s="2" t="s">
         <v>31</v>
@@ -10722,7 +10721,7 @@
       <c r="AB87" s="2"/>
       <c r="AC87" s="2"/>
     </row>
-    <row r="88" spans="1:29" ht="23.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:29" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A88" s="2">
         <v>87</v>
       </c>
@@ -10766,7 +10765,7 @@
       <c r="O88" s="2"/>
       <c r="P88" s="2"/>
       <c r="Q88" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="R88" s="2" t="s">
         <v>31</v>
@@ -10783,7 +10782,7 @@
       <c r="AB88" s="2"/>
       <c r="AC88" s="2"/>
     </row>
-    <row r="89" spans="1:29" ht="23.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:29" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A89" s="2">
         <v>88</v>
       </c>
@@ -10827,7 +10826,7 @@
       <c r="O89" s="2"/>
       <c r="P89" s="2"/>
       <c r="Q89" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="R89" s="2" t="s">
         <v>31</v>
@@ -10844,7 +10843,7 @@
       <c r="AB89" s="2"/>
       <c r="AC89" s="2"/>
     </row>
-    <row r="90" spans="1:29" ht="23.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:29" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A90" s="2">
         <v>89</v>
       </c>
@@ -10888,7 +10887,7 @@
       <c r="O90" s="2"/>
       <c r="P90" s="2"/>
       <c r="Q90" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="R90" s="2" t="s">
         <v>31</v>
@@ -10905,7 +10904,7 @@
       <c r="AB90" s="2"/>
       <c r="AC90" s="2"/>
     </row>
-    <row r="91" spans="1:29" ht="23.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:29" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A91" s="2">
         <v>90</v>
       </c>
@@ -10949,7 +10948,7 @@
       <c r="O91" s="2"/>
       <c r="P91" s="2"/>
       <c r="Q91" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="R91" s="2" t="s">
         <v>31</v>
@@ -10966,7 +10965,7 @@
       <c r="AB91" s="2"/>
       <c r="AC91" s="2"/>
     </row>
-    <row r="92" spans="1:29" ht="23.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:29" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A92" s="2">
         <v>91</v>
       </c>
@@ -11010,7 +11009,7 @@
       <c r="O92" s="2"/>
       <c r="P92" s="2"/>
       <c r="Q92" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="R92" s="2" t="s">
         <v>31</v>
@@ -11027,7 +11026,7 @@
       <c r="AB92" s="2"/>
       <c r="AC92" s="2"/>
     </row>
-    <row r="93" spans="1:29" ht="23.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:29" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A93" s="2">
         <v>92</v>
       </c>
@@ -11071,7 +11070,7 @@
       <c r="O93" s="2"/>
       <c r="P93" s="2"/>
       <c r="Q93" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="R93" s="2" t="s">
         <v>28</v>
@@ -11088,7 +11087,7 @@
       <c r="AB93" s="2"/>
       <c r="AC93" s="2"/>
     </row>
-    <row r="94" spans="1:29" ht="23.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:29" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A94" s="2">
         <v>93</v>
       </c>
@@ -11132,7 +11131,7 @@
       <c r="O94" s="2"/>
       <c r="P94" s="2"/>
       <c r="Q94" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="R94" s="2" t="s">
         <v>31</v>
@@ -11149,7 +11148,7 @@
       <c r="AB94" s="2"/>
       <c r="AC94" s="2"/>
     </row>
-    <row r="95" spans="1:29" ht="23.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:29" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A95" s="2">
         <v>94</v>
       </c>
@@ -11193,7 +11192,7 @@
       <c r="O95" s="2"/>
       <c r="P95" s="2"/>
       <c r="Q95" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="R95" s="2" t="s">
         <v>31</v>
@@ -11210,7 +11209,7 @@
       <c r="AB95" s="2"/>
       <c r="AC95" s="2"/>
     </row>
-    <row r="96" spans="1:29" ht="23.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:29" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A96" s="2">
         <v>95</v>
       </c>
@@ -11254,7 +11253,7 @@
       <c r="O96" s="2"/>
       <c r="P96" s="2"/>
       <c r="Q96" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="R96" s="2" t="s">
         <v>31</v>
@@ -11271,7 +11270,7 @@
       <c r="AB96" s="2"/>
       <c r="AC96" s="2"/>
     </row>
-    <row r="97" spans="1:29" ht="23.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:29" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A97" s="2">
         <v>96</v>
       </c>
@@ -11315,7 +11314,7 @@
       <c r="O97" s="2"/>
       <c r="P97" s="2"/>
       <c r="Q97" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="R97" s="2" t="s">
         <v>31</v>
@@ -11332,7 +11331,7 @@
       <c r="AB97" s="2"/>
       <c r="AC97" s="2"/>
     </row>
-    <row r="98" spans="1:29" ht="23.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:29" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A98" s="2">
         <v>97</v>
       </c>
@@ -11376,7 +11375,7 @@
       <c r="O98" s="2"/>
       <c r="P98" s="2"/>
       <c r="Q98" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="R98" s="2" t="s">
         <v>31</v>
@@ -11393,7 +11392,7 @@
       <c r="AB98" s="2"/>
       <c r="AC98" s="2"/>
     </row>
-    <row r="99" spans="1:29" ht="23.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:29" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A99" s="2">
         <v>98</v>
       </c>
@@ -11437,7 +11436,7 @@
       <c r="O99" s="2"/>
       <c r="P99" s="2"/>
       <c r="Q99" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="R99" s="2" t="s">
         <v>31</v>
@@ -11454,7 +11453,7 @@
       <c r="AB99" s="2"/>
       <c r="AC99" s="2"/>
     </row>
-    <row r="100" spans="1:29" ht="23.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:29" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A100" s="2">
         <v>99</v>
       </c>
@@ -11498,7 +11497,7 @@
       <c r="O100" s="2"/>
       <c r="P100" s="2"/>
       <c r="Q100" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="R100" s="2" t="s">
         <v>31</v>
@@ -11515,7 +11514,7 @@
       <c r="AB100" s="2"/>
       <c r="AC100" s="2"/>
     </row>
-    <row r="101" spans="1:29" ht="23.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:29" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A101" s="2">
         <v>100</v>
       </c>
@@ -11559,7 +11558,7 @@
       <c r="O101" s="2"/>
       <c r="P101" s="2"/>
       <c r="Q101" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="R101" s="2" t="s">
         <v>31</v>
@@ -11576,7 +11575,7 @@
       <c r="AB101" s="2"/>
       <c r="AC101" s="2"/>
     </row>
-    <row r="102" spans="1:29" ht="23.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:29" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A102" s="2">
         <v>101</v>
       </c>
@@ -11620,7 +11619,7 @@
       <c r="O102" s="2"/>
       <c r="P102" s="2"/>
       <c r="Q102" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="R102" s="2" t="s">
         <v>31</v>
@@ -11637,7 +11636,7 @@
       <c r="AB102" s="2"/>
       <c r="AC102" s="2"/>
     </row>
-    <row r="103" spans="1:29" ht="23.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:29" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A103" s="2">
         <v>102</v>
       </c>
@@ -11681,7 +11680,7 @@
       <c r="O103" s="2"/>
       <c r="P103" s="2"/>
       <c r="Q103" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="R103" s="2" t="s">
         <v>31</v>
@@ -11698,7 +11697,7 @@
       <c r="AB103" s="2"/>
       <c r="AC103" s="2"/>
     </row>
-    <row r="104" spans="1:29" ht="23.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:29" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A104" s="2">
         <v>103</v>
       </c>
@@ -11742,7 +11741,7 @@
       <c r="O104" s="2"/>
       <c r="P104" s="2"/>
       <c r="Q104" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="R104" s="2" t="s">
         <v>31</v>
@@ -11759,7 +11758,7 @@
       <c r="AB104" s="2"/>
       <c r="AC104" s="2"/>
     </row>
-    <row r="105" spans="1:29" ht="23.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:29" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A105" s="2">
         <v>104</v>
       </c>
@@ -11803,7 +11802,7 @@
       <c r="O105" s="2"/>
       <c r="P105" s="2"/>
       <c r="Q105" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="R105" s="2" t="s">
         <v>28</v>
@@ -11820,7 +11819,7 @@
       <c r="AB105" s="2"/>
       <c r="AC105" s="2"/>
     </row>
-    <row r="106" spans="1:29" ht="23.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:29" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A106" s="2">
         <v>105</v>
       </c>
@@ -11864,7 +11863,7 @@
       <c r="O106" s="2"/>
       <c r="P106" s="2"/>
       <c r="Q106" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="R106" s="2" t="s">
         <v>28</v>
@@ -11881,7 +11880,7 @@
       <c r="AB106" s="2"/>
       <c r="AC106" s="2"/>
     </row>
-    <row r="107" spans="1:29" ht="23.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:29" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A107" s="2">
         <v>106</v>
       </c>
@@ -11925,7 +11924,7 @@
       <c r="O107" s="2"/>
       <c r="P107" s="2"/>
       <c r="Q107" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="R107" s="2" t="s">
         <v>31</v>
@@ -11942,7 +11941,7 @@
       <c r="AB107" s="2"/>
       <c r="AC107" s="2"/>
     </row>
-    <row r="108" spans="1:29" ht="23.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:29" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A108" s="2">
         <v>107</v>
       </c>
@@ -11986,7 +11985,7 @@
       <c r="O108" s="2"/>
       <c r="P108" s="2"/>
       <c r="Q108" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="R108" s="2" t="s">
         <v>28</v>
@@ -12003,7 +12002,7 @@
       <c r="AB108" s="2"/>
       <c r="AC108" s="2"/>
     </row>
-    <row r="109" spans="1:29" ht="23.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:29" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A109" s="2">
         <v>108</v>
       </c>
@@ -12047,7 +12046,7 @@
       <c r="O109" s="2"/>
       <c r="P109" s="2"/>
       <c r="Q109" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="R109" s="2" t="s">
         <v>28</v>
@@ -12064,7 +12063,7 @@
       <c r="AB109" s="2"/>
       <c r="AC109" s="2"/>
     </row>
-    <row r="110" spans="1:29" ht="23.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:29" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A110" s="2">
         <v>109</v>
       </c>
@@ -12108,7 +12107,7 @@
       <c r="O110" s="2"/>
       <c r="P110" s="2"/>
       <c r="Q110" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="R110" s="2" t="s">
         <v>31</v>
@@ -12125,7 +12124,7 @@
       <c r="AB110" s="2"/>
       <c r="AC110" s="2"/>
     </row>
-    <row r="111" spans="1:29" ht="23.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:29" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A111" s="2">
         <v>110</v>
       </c>
@@ -12169,7 +12168,7 @@
       <c r="O111" s="2"/>
       <c r="P111" s="2"/>
       <c r="Q111" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="R111" s="2" t="s">
         <v>28</v>
@@ -12186,7 +12185,7 @@
       <c r="AB111" s="2"/>
       <c r="AC111" s="2"/>
     </row>
-    <row r="112" spans="1:29" ht="23.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:29" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A112" s="2">
         <v>111</v>
       </c>
@@ -12230,7 +12229,7 @@
       <c r="O112" s="2"/>
       <c r="P112" s="2"/>
       <c r="Q112" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="R112" s="2" t="s">
         <v>28</v>
@@ -12247,7 +12246,7 @@
       <c r="AB112" s="2"/>
       <c r="AC112" s="2"/>
     </row>
-    <row r="113" spans="1:29" ht="23.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:29" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A113" s="2">
         <v>112</v>
       </c>
@@ -12291,7 +12290,7 @@
       <c r="O113" s="2"/>
       <c r="P113" s="2"/>
       <c r="Q113" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="R113" s="2" t="s">
         <v>28</v>
@@ -12308,7 +12307,7 @@
       <c r="AB113" s="2"/>
       <c r="AC113" s="2"/>
     </row>
-    <row r="114" spans="1:29" ht="23.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:29" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A114" s="2">
         <v>113</v>
       </c>
@@ -12352,7 +12351,7 @@
       <c r="O114" s="2"/>
       <c r="P114" s="2"/>
       <c r="Q114" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="R114" s="2" t="s">
         <v>31</v>
@@ -12369,7 +12368,7 @@
       <c r="AB114" s="2"/>
       <c r="AC114" s="2"/>
     </row>
-    <row r="115" spans="1:29" ht="23.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:29" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A115" s="2">
         <v>114</v>
       </c>
@@ -12413,7 +12412,7 @@
       <c r="O115" s="2"/>
       <c r="P115" s="2"/>
       <c r="Q115" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="R115" s="2" t="s">
         <v>31</v>
@@ -12430,7 +12429,7 @@
       <c r="AB115" s="2"/>
       <c r="AC115" s="2"/>
     </row>
-    <row r="116" spans="1:29" ht="23.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:29" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A116" s="2">
         <v>115</v>
       </c>
@@ -12474,7 +12473,7 @@
       <c r="O116" s="2"/>
       <c r="P116" s="2"/>
       <c r="Q116" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="R116" s="2" t="s">
         <v>31</v>
@@ -12491,7 +12490,7 @@
       <c r="AB116" s="2"/>
       <c r="AC116" s="2"/>
     </row>
-    <row r="117" spans="1:29" ht="23.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:29" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A117" s="2">
         <v>116</v>
       </c>
@@ -12535,7 +12534,7 @@
       <c r="O117" s="2"/>
       <c r="P117" s="2"/>
       <c r="Q117" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="R117" s="2" t="s">
         <v>31</v>
@@ -12552,7 +12551,7 @@
       <c r="AB117" s="2"/>
       <c r="AC117" s="2"/>
     </row>
-    <row r="118" spans="1:29" ht="23.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:29" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A118" s="2">
         <v>117</v>
       </c>
@@ -12596,7 +12595,7 @@
       <c r="O118" s="2"/>
       <c r="P118" s="2"/>
       <c r="Q118" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="R118" s="2" t="s">
         <v>31</v>
@@ -12613,7 +12612,7 @@
       <c r="AB118" s="2"/>
       <c r="AC118" s="2"/>
     </row>
-    <row r="119" spans="1:29" ht="23.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:29" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A119" s="2">
         <v>118</v>
       </c>
@@ -12657,7 +12656,7 @@
       <c r="O119" s="2"/>
       <c r="P119" s="2"/>
       <c r="Q119" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="R119" s="2" t="s">
         <v>31</v>
@@ -12674,7 +12673,7 @@
       <c r="AB119" s="2"/>
       <c r="AC119" s="2"/>
     </row>
-    <row r="120" spans="1:29" ht="23.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:29" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A120" s="2">
         <v>119</v>
       </c>
@@ -12735,7 +12734,7 @@
       <c r="AB120" s="2"/>
       <c r="AC120" s="2"/>
     </row>
-    <row r="121" spans="1:29" ht="23.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:29" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A121" s="2">
         <v>120</v>
       </c>
@@ -12796,7 +12795,7 @@
       <c r="AB121" s="2"/>
       <c r="AC121" s="2"/>
     </row>
-    <row r="122" spans="1:29" ht="23.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:29" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A122" s="2">
         <v>121</v>
       </c>
@@ -12857,7 +12856,7 @@
       <c r="AB122" s="2"/>
       <c r="AC122" s="2"/>
     </row>
-    <row r="123" spans="1:29" ht="23.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:29" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A123" s="2">
         <v>122</v>
       </c>
@@ -12918,7 +12917,7 @@
       <c r="AB123" s="2"/>
       <c r="AC123" s="2"/>
     </row>
-    <row r="124" spans="1:29" ht="23.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:29" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A124" s="2">
         <v>123</v>
       </c>
@@ -12979,7 +12978,7 @@
       <c r="AB124" s="2"/>
       <c r="AC124" s="2"/>
     </row>
-    <row r="125" spans="1:29" ht="23.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:29" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A125" s="2">
         <v>124</v>
       </c>
@@ -13040,7 +13039,7 @@
       <c r="AB125" s="2"/>
       <c r="AC125" s="2"/>
     </row>
-    <row r="126" spans="1:29" ht="23.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:29" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A126" s="2">
         <v>125</v>
       </c>
@@ -13101,7 +13100,7 @@
       <c r="AB126" s="2"/>
       <c r="AC126" s="2"/>
     </row>
-    <row r="127" spans="1:29" ht="23.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:29" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A127" s="2">
         <v>126</v>
       </c>
@@ -13162,7 +13161,7 @@
       <c r="AB127" s="2"/>
       <c r="AC127" s="2"/>
     </row>
-    <row r="128" spans="1:29" ht="23.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:29" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A128" s="2">
         <v>127</v>
       </c>
@@ -13223,7 +13222,7 @@
       <c r="AB128" s="2"/>
       <c r="AC128" s="2"/>
     </row>
-    <row r="129" spans="1:29" ht="23.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:29" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A129" s="2">
         <v>128</v>
       </c>
@@ -13284,7 +13283,7 @@
       <c r="AB129" s="2"/>
       <c r="AC129" s="2"/>
     </row>
-    <row r="130" spans="1:29" ht="23.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:29" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A130" s="2">
         <v>129</v>
       </c>
@@ -13345,7 +13344,7 @@
       <c r="AB130" s="2"/>
       <c r="AC130" s="2"/>
     </row>
-    <row r="131" spans="1:29" ht="23.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:29" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A131" s="2">
         <v>130</v>
       </c>
@@ -13467,7 +13466,7 @@
       <c r="AB132" s="2"/>
       <c r="AC132" s="2"/>
     </row>
-    <row r="133" spans="1:29" ht="23.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:29" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A133" s="2">
         <v>132</v>
       </c>
@@ -13528,7 +13527,7 @@
       <c r="AB133" s="2"/>
       <c r="AC133" s="2"/>
     </row>
-    <row r="134" spans="1:29" ht="23.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:29" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A134" s="2">
         <v>133</v>
       </c>
@@ -13589,7 +13588,7 @@
       <c r="AB134" s="2"/>
       <c r="AC134" s="2"/>
     </row>
-    <row r="135" spans="1:29" ht="23.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:29" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A135" s="2">
         <v>134</v>
       </c>
@@ -13650,7 +13649,7 @@
       <c r="AB135" s="2"/>
       <c r="AC135" s="2"/>
     </row>
-    <row r="136" spans="1:29" ht="23.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:29" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A136" s="2">
         <v>135</v>
       </c>
@@ -13711,7 +13710,7 @@
       <c r="AB136" s="2"/>
       <c r="AC136" s="2"/>
     </row>
-    <row r="137" spans="1:29" ht="23.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="137" spans="1:29" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A137" s="2">
         <v>136</v>
       </c>
@@ -13772,7 +13771,7 @@
       <c r="AB137" s="2"/>
       <c r="AC137" s="2"/>
     </row>
-    <row r="138" spans="1:29" ht="23.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:29" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A138" s="2">
         <v>137</v>
       </c>
@@ -13833,7 +13832,7 @@
       <c r="AB138" s="2"/>
       <c r="AC138" s="2"/>
     </row>
-    <row r="139" spans="1:29" ht="23.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="139" spans="1:29" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A139" s="2">
         <v>138</v>
       </c>
@@ -13955,7 +13954,7 @@
       <c r="AB140" s="2"/>
       <c r="AC140" s="2"/>
     </row>
-    <row r="141" spans="1:29" ht="23.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="141" spans="1:29" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A141" s="2">
         <v>140</v>
       </c>
@@ -14077,7 +14076,7 @@
       <c r="AB142" s="2"/>
       <c r="AC142" s="2"/>
     </row>
-    <row r="143" spans="1:29" ht="23.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="143" spans="1:29" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A143" s="2">
         <v>142</v>
       </c>
@@ -14138,7 +14137,7 @@
       <c r="AB143" s="2"/>
       <c r="AC143" s="2"/>
     </row>
-    <row r="144" spans="1:29" ht="23.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="144" spans="1:29" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A144" s="2">
         <v>143</v>
       </c>
@@ -14199,7 +14198,7 @@
       <c r="AB144" s="2"/>
       <c r="AC144" s="2"/>
     </row>
-    <row r="145" spans="1:29" ht="23.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="145" spans="1:29" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A145" s="2">
         <v>144</v>
       </c>
@@ -14260,7 +14259,7 @@
       <c r="AB145" s="2"/>
       <c r="AC145" s="2"/>
     </row>
-    <row r="146" spans="1:29" ht="23.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="146" spans="1:29" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A146" s="2">
         <v>145</v>
       </c>
@@ -14321,7 +14320,7 @@
       <c r="AB146" s="2"/>
       <c r="AC146" s="2"/>
     </row>
-    <row r="147" spans="1:29" ht="23.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="147" spans="1:29" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A147" s="2">
         <v>146</v>
       </c>
@@ -14382,7 +14381,7 @@
       <c r="AB147" s="2"/>
       <c r="AC147" s="2"/>
     </row>
-    <row r="148" spans="1:29" ht="23.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="148" spans="1:29" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A148" s="2">
         <v>147</v>
       </c>
@@ -14443,7 +14442,7 @@
       <c r="AB148" s="2"/>
       <c r="AC148" s="2"/>
     </row>
-    <row r="149" spans="1:29" ht="23.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="149" spans="1:29" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A149" s="2">
         <v>148</v>
       </c>
@@ -14565,7 +14564,7 @@
       <c r="AB150" s="2"/>
       <c r="AC150" s="2"/>
     </row>
-    <row r="151" spans="1:29" ht="23.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="151" spans="1:29" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A151" s="2">
         <v>150</v>
       </c>
@@ -14687,7 +14686,7 @@
       <c r="AB152" s="2"/>
       <c r="AC152" s="2"/>
     </row>
-    <row r="153" spans="1:29" ht="23.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="153" spans="1:29" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A153" s="2">
         <v>152</v>
       </c>
@@ -14748,7 +14747,7 @@
       <c r="AB153" s="2"/>
       <c r="AC153" s="2"/>
     </row>
-    <row r="154" spans="1:29" ht="23.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="154" spans="1:29" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A154" s="2">
         <v>153</v>
       </c>
@@ -14809,7 +14808,7 @@
       <c r="AB154" s="2"/>
       <c r="AC154" s="2"/>
     </row>
-    <row r="155" spans="1:29" ht="23.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="155" spans="1:29" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A155" s="2">
         <v>154</v>
       </c>
@@ -14870,7 +14869,7 @@
       <c r="AB155" s="2"/>
       <c r="AC155" s="2"/>
     </row>
-    <row r="156" spans="1:29" ht="23.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="156" spans="1:29" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A156" s="2">
         <v>155</v>
       </c>
@@ -14992,7 +14991,7 @@
       <c r="AB157" s="2"/>
       <c r="AC157" s="2"/>
     </row>
-    <row r="158" spans="1:29" ht="23.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="158" spans="1:29" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A158" s="2">
         <v>157</v>
       </c>
@@ -15053,7 +15052,7 @@
       <c r="AB158" s="2"/>
       <c r="AC158" s="2"/>
     </row>
-    <row r="159" spans="1:29" ht="23.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="159" spans="1:29" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A159" s="2">
         <v>158</v>
       </c>
@@ -15114,7 +15113,7 @@
       <c r="AB159" s="2"/>
       <c r="AC159" s="2"/>
     </row>
-    <row r="160" spans="1:29" ht="23.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="160" spans="1:29" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A160" s="2">
         <v>159</v>
       </c>
@@ -15175,7 +15174,7 @@
       <c r="AB160" s="2"/>
       <c r="AC160" s="2"/>
     </row>
-    <row r="161" spans="1:29" ht="23.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="161" spans="1:29" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A161" s="2">
         <v>160</v>
       </c>
@@ -15236,7 +15235,7 @@
       <c r="AB161" s="2"/>
       <c r="AC161" s="2"/>
     </row>
-    <row r="162" spans="1:29" ht="23.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="162" spans="1:29" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A162" s="2">
         <v>161</v>
       </c>
@@ -15297,7 +15296,7 @@
       <c r="AB162" s="2"/>
       <c r="AC162" s="2"/>
     </row>
-    <row r="163" spans="1:29" ht="23.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="163" spans="1:29" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A163" s="2">
         <v>162</v>
       </c>
@@ -15358,7 +15357,7 @@
       <c r="AB163" s="2"/>
       <c r="AC163" s="2"/>
     </row>
-    <row r="164" spans="1:29" ht="23.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="164" spans="1:29" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A164" s="2">
         <v>163</v>
       </c>
@@ -15419,7 +15418,7 @@
       <c r="AB164" s="2"/>
       <c r="AC164" s="2"/>
     </row>
-    <row r="165" spans="1:29" ht="23.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="165" spans="1:29" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A165" s="2">
         <v>164</v>
       </c>
@@ -15480,7 +15479,7 @@
       <c r="AB165" s="2"/>
       <c r="AC165" s="2"/>
     </row>
-    <row r="166" spans="1:29" ht="23.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="166" spans="1:29" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A166" s="2">
         <v>165</v>
       </c>
@@ -15541,7 +15540,7 @@
       <c r="AB166" s="2"/>
       <c r="AC166" s="2"/>
     </row>
-    <row r="167" spans="1:29" ht="23.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="167" spans="1:29" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A167" s="2">
         <v>166</v>
       </c>
@@ -15602,7 +15601,7 @@
       <c r="AB167" s="2"/>
       <c r="AC167" s="2"/>
     </row>
-    <row r="168" spans="1:29" ht="23.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="168" spans="1:29" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A168" s="2">
         <v>167</v>
       </c>
@@ -15663,7 +15662,7 @@
       <c r="AB168" s="2"/>
       <c r="AC168" s="2"/>
     </row>
-    <row r="169" spans="1:29" ht="23.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="169" spans="1:29" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A169" s="2">
         <v>168</v>
       </c>
@@ -15724,7 +15723,7 @@
       <c r="AB169" s="2"/>
       <c r="AC169" s="2"/>
     </row>
-    <row r="170" spans="1:29" ht="23.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="170" spans="1:29" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A170" s="2">
         <v>169</v>
       </c>
@@ -15785,7 +15784,7 @@
       <c r="AB170" s="2"/>
       <c r="AC170" s="2"/>
     </row>
-    <row r="171" spans="1:29" ht="23.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="171" spans="1:29" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A171" s="2">
         <v>170</v>
       </c>
@@ -15846,7 +15845,7 @@
       <c r="AB171" s="2"/>
       <c r="AC171" s="2"/>
     </row>
-    <row r="172" spans="1:29" ht="23.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="172" spans="1:29" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A172" s="2">
         <v>171</v>
       </c>
@@ -15907,7 +15906,7 @@
       <c r="AB172" s="2"/>
       <c r="AC172" s="2"/>
     </row>
-    <row r="173" spans="1:29" ht="23.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="173" spans="1:29" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A173" s="2">
         <v>172</v>
       </c>
@@ -15968,7 +15967,7 @@
       <c r="AB173" s="2"/>
       <c r="AC173" s="2"/>
     </row>
-    <row r="174" spans="1:29" ht="23.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="174" spans="1:29" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A174" s="2">
         <v>173</v>
       </c>
@@ -16273,7 +16272,7 @@
       <c r="AB178" s="2"/>
       <c r="AC178" s="2"/>
     </row>
-    <row r="179" spans="1:29" ht="23.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="179" spans="1:29" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A179" s="2">
         <v>178</v>
       </c>
@@ -16883,7 +16882,7 @@
       <c r="AB188" s="2"/>
       <c r="AC188" s="2"/>
     </row>
-    <row r="189" spans="1:29" ht="23.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="189" spans="1:29" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A189" s="2">
         <v>188</v>
       </c>
@@ -17005,7 +17004,7 @@
       <c r="AB190" s="2"/>
       <c r="AC190" s="2"/>
     </row>
-    <row r="191" spans="1:29" ht="23.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="191" spans="1:29" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A191" s="2">
         <v>190</v>
       </c>
@@ -17066,7 +17065,7 @@
       <c r="AB191" s="2"/>
       <c r="AC191" s="2"/>
     </row>
-    <row r="192" spans="1:29" ht="23.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="192" spans="1:29" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A192" s="2">
         <v>191</v>
       </c>
@@ -17310,7 +17309,7 @@
       <c r="AB195" s="2"/>
       <c r="AC195" s="2"/>
     </row>
-    <row r="196" spans="1:29" ht="23.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="196" spans="1:29" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A196" s="2">
         <v>195</v>
       </c>
@@ -17371,7 +17370,7 @@
       <c r="AB196" s="2"/>
       <c r="AC196" s="2"/>
     </row>
-    <row r="197" spans="1:29" ht="23.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="197" spans="1:29" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A197" s="2">
         <v>196</v>
       </c>
@@ -17432,7 +17431,7 @@
       <c r="AB197" s="2"/>
       <c r="AC197" s="2"/>
     </row>
-    <row r="198" spans="1:29" ht="23.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="198" spans="1:29" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A198" s="2">
         <v>197</v>
       </c>
@@ -17493,7 +17492,7 @@
       <c r="AB198" s="2"/>
       <c r="AC198" s="2"/>
     </row>
-    <row r="199" spans="1:29" ht="23.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="199" spans="1:29" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A199" s="2">
         <v>198</v>
       </c>
@@ -17554,7 +17553,7 @@
       <c r="AB199" s="2"/>
       <c r="AC199" s="2"/>
     </row>
-    <row r="200" spans="1:29" ht="23.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="200" spans="1:29" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A200" s="2">
         <v>199</v>
       </c>
@@ -17737,7 +17736,7 @@
       <c r="AB202" s="2"/>
       <c r="AC202" s="2"/>
     </row>
-    <row r="203" spans="1:29" ht="23.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="203" spans="1:29" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A203" s="2">
         <v>202</v>
       </c>
@@ -17798,7 +17797,7 @@
       <c r="AB203" s="2"/>
       <c r="AC203" s="2"/>
     </row>
-    <row r="204" spans="1:29" ht="23.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="204" spans="1:29" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A204" s="2">
         <v>203</v>
       </c>
@@ -17859,7 +17858,7 @@
       <c r="AB204" s="2"/>
       <c r="AC204" s="2"/>
     </row>
-    <row r="205" spans="1:29" ht="23.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="205" spans="1:29" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A205" s="2">
         <v>204</v>
       </c>
@@ -17920,7 +17919,7 @@
       <c r="AB205" s="2"/>
       <c r="AC205" s="2"/>
     </row>
-    <row r="206" spans="1:29" ht="23.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="206" spans="1:29" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A206" s="2">
         <v>205</v>
       </c>
@@ -18103,7 +18102,7 @@
       <c r="AB208" s="2"/>
       <c r="AC208" s="2"/>
     </row>
-    <row r="209" spans="1:29" ht="23.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="209" spans="1:29" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A209" s="2">
         <v>208</v>
       </c>
@@ -18164,7 +18163,7 @@
       <c r="AB209" s="2"/>
       <c r="AC209" s="2"/>
     </row>
-    <row r="210" spans="1:29" ht="23.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="210" spans="1:29" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A210" s="2">
         <v>209</v>
       </c>
@@ -18225,7 +18224,7 @@
       <c r="AB210" s="2"/>
       <c r="AC210" s="2"/>
     </row>
-    <row r="211" spans="1:29" ht="23.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="211" spans="1:29" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A211" s="2">
         <v>210</v>
       </c>
@@ -18286,7 +18285,7 @@
       <c r="AB211" s="2"/>
       <c r="AC211" s="2"/>
     </row>
-    <row r="212" spans="1:29" ht="23.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="212" spans="1:29" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A212" s="2">
         <v>211</v>
       </c>
@@ -18408,7 +18407,7 @@
       <c r="AB213" s="2"/>
       <c r="AC213" s="2"/>
     </row>
-    <row r="214" spans="1:29" ht="23.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="214" spans="1:29" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A214" s="2">
         <v>213</v>
       </c>
@@ -18469,7 +18468,7 @@
       <c r="AB214" s="2"/>
       <c r="AC214" s="2"/>
     </row>
-    <row r="215" spans="1:29" ht="23.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="215" spans="1:29" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A215" s="2">
         <v>214</v>
       </c>
@@ -18530,7 +18529,7 @@
       <c r="AB215" s="2"/>
       <c r="AC215" s="2"/>
     </row>
-    <row r="216" spans="1:29" ht="23.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="216" spans="1:29" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A216" s="2">
         <v>215</v>
       </c>
@@ -18591,7 +18590,7 @@
       <c r="AB216" s="2"/>
       <c r="AC216" s="2"/>
     </row>
-    <row r="217" spans="1:29" ht="23.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="217" spans="1:29" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A217" s="2">
         <v>216</v>
       </c>
@@ -18652,7 +18651,7 @@
       <c r="AB217" s="2"/>
       <c r="AC217" s="2"/>
     </row>
-    <row r="218" spans="1:29" ht="23.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="218" spans="1:29" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A218" s="2">
         <v>217</v>
       </c>
@@ -18713,7 +18712,7 @@
       <c r="AB218" s="2"/>
       <c r="AC218" s="2"/>
     </row>
-    <row r="219" spans="1:29" ht="23.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="219" spans="1:29" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A219" s="2">
         <v>218</v>
       </c>
@@ -18774,7 +18773,7 @@
       <c r="AB219" s="2"/>
       <c r="AC219" s="2"/>
     </row>
-    <row r="220" spans="1:29" ht="23.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="220" spans="1:29" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A220" s="2">
         <v>219</v>
       </c>
@@ -18835,7 +18834,7 @@
       <c r="AB220" s="2"/>
       <c r="AC220" s="2"/>
     </row>
-    <row r="221" spans="1:29" ht="23.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="221" spans="1:29" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A221" s="2">
         <v>220</v>
       </c>
@@ -18896,7 +18895,7 @@
       <c r="AB221" s="2"/>
       <c r="AC221" s="2"/>
     </row>
-    <row r="222" spans="1:29" ht="23.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="222" spans="1:29" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A222" s="2">
         <v>221</v>
       </c>
@@ -18957,7 +18956,7 @@
       <c r="AB222" s="2"/>
       <c r="AC222" s="2"/>
     </row>
-    <row r="223" spans="1:29" ht="23.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="223" spans="1:29" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A223" s="2">
         <v>222</v>
       </c>
@@ -19018,7 +19017,7 @@
       <c r="AB223" s="2"/>
       <c r="AC223" s="2"/>
     </row>
-    <row r="224" spans="1:29" ht="23.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="224" spans="1:29" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A224" s="2">
         <v>223</v>
       </c>
@@ -19079,7 +19078,7 @@
       <c r="AB224" s="2"/>
       <c r="AC224" s="2"/>
     </row>
-    <row r="225" spans="1:29" ht="23.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="225" spans="1:29" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A225" s="2">
         <v>224</v>
       </c>
@@ -19262,7 +19261,7 @@
       <c r="AB227" s="2"/>
       <c r="AC227" s="2"/>
     </row>
-    <row r="228" spans="1:29" ht="23.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="228" spans="1:29" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A228" s="2">
         <v>227</v>
       </c>
@@ -19323,7 +19322,7 @@
       <c r="AB228" s="2"/>
       <c r="AC228" s="2"/>
     </row>
-    <row r="229" spans="1:29" ht="23.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="229" spans="1:29" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A229" s="2">
         <v>228</v>
       </c>
@@ -19445,7 +19444,7 @@
       <c r="AB230" s="2"/>
       <c r="AC230" s="2"/>
     </row>
-    <row r="231" spans="1:29" ht="23.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="231" spans="1:29" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A231" s="2">
         <v>230</v>
       </c>
@@ -19567,7 +19566,7 @@
       <c r="AB232" s="2"/>
       <c r="AC232" s="2"/>
     </row>
-    <row r="233" spans="1:29" ht="23.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="233" spans="1:29" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A233" s="2">
         <v>232</v>
       </c>
@@ -19689,7 +19688,7 @@
       <c r="AB234" s="2"/>
       <c r="AC234" s="2"/>
     </row>
-    <row r="235" spans="1:29" ht="23.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="235" spans="1:29" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A235" s="2">
         <v>234</v>
       </c>
@@ -19750,7 +19749,7 @@
       <c r="AB235" s="2"/>
       <c r="AC235" s="2"/>
     </row>
-    <row r="236" spans="1:29" ht="23.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="236" spans="1:29" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A236" s="2">
         <v>235</v>
       </c>
@@ -19811,7 +19810,7 @@
       <c r="AB236" s="2"/>
       <c r="AC236" s="2"/>
     </row>
-    <row r="237" spans="1:29" ht="23.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="237" spans="1:29" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A237" s="2">
         <v>236</v>
       </c>
@@ -19872,7 +19871,7 @@
       <c r="AB237" s="2"/>
       <c r="AC237" s="2"/>
     </row>
-    <row r="238" spans="1:29" ht="23.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="238" spans="1:29" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A238" s="2">
         <v>237</v>
       </c>
@@ -19994,7 +19993,7 @@
       <c r="AB239" s="2"/>
       <c r="AC239" s="2"/>
     </row>
-    <row r="240" spans="1:29" ht="23.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="240" spans="1:29" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A240" s="2">
         <v>239</v>
       </c>
@@ -20116,7 +20115,7 @@
       <c r="AB241" s="2"/>
       <c r="AC241" s="2"/>
     </row>
-    <row r="242" spans="1:29" ht="23.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="242" spans="1:29" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A242" s="2">
         <v>241</v>
       </c>
@@ -20177,7 +20176,7 @@
       <c r="AB242" s="2"/>
       <c r="AC242" s="2"/>
     </row>
-    <row r="243" spans="1:29" ht="23.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="243" spans="1:29" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A243" s="2">
         <v>242</v>
       </c>
@@ -20238,7 +20237,7 @@
       <c r="AB243" s="2"/>
       <c r="AC243" s="2"/>
     </row>
-    <row r="244" spans="1:29" ht="23.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="244" spans="1:29" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A244" s="2">
         <v>243</v>
       </c>
@@ -20421,7 +20420,7 @@
       <c r="AB246" s="2"/>
       <c r="AC246" s="2"/>
     </row>
-    <row r="247" spans="1:29" ht="23.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="247" spans="1:29" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A247" s="2">
         <v>246</v>
       </c>
@@ -20482,7 +20481,7 @@
       <c r="AB247" s="2"/>
       <c r="AC247" s="2"/>
     </row>
-    <row r="248" spans="1:29" ht="23.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="248" spans="1:29" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A248" s="2">
         <v>247</v>
       </c>
@@ -20543,7 +20542,7 @@
       <c r="AB248" s="2"/>
       <c r="AC248" s="2"/>
     </row>
-    <row r="249" spans="1:29" ht="23.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="249" spans="1:29" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A249" s="2">
         <v>248</v>
       </c>
@@ -20604,7 +20603,7 @@
       <c r="AB249" s="2"/>
       <c r="AC249" s="2"/>
     </row>
-    <row r="250" spans="1:29" ht="23.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="250" spans="1:29" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A250" s="2">
         <v>249</v>
       </c>
@@ -20665,7 +20664,7 @@
       <c r="AB250" s="2"/>
       <c r="AC250" s="2"/>
     </row>
-    <row r="251" spans="1:29" ht="23.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="251" spans="1:29" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A251" s="2">
         <v>250</v>
       </c>
@@ -20726,7 +20725,7 @@
       <c r="AB251" s="2"/>
       <c r="AC251" s="2"/>
     </row>
-    <row r="252" spans="1:29" ht="23.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="252" spans="1:29" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A252" s="2">
         <v>251</v>
       </c>
@@ -20787,7 +20786,7 @@
       <c r="AB252" s="2"/>
       <c r="AC252" s="2"/>
     </row>
-    <row r="253" spans="1:29" ht="23.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="253" spans="1:29" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A253" s="2">
         <v>252</v>
       </c>
@@ -20848,7 +20847,7 @@
       <c r="AB253" s="2"/>
       <c r="AC253" s="2"/>
     </row>
-    <row r="254" spans="1:29" ht="23.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="254" spans="1:29" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A254" s="2">
         <v>253</v>
       </c>
@@ -20909,7 +20908,7 @@
       <c r="AB254" s="2"/>
       <c r="AC254" s="2"/>
     </row>
-    <row r="255" spans="1:29" ht="23.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="255" spans="1:29" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A255" s="2">
         <v>254</v>
       </c>
@@ -20970,7 +20969,7 @@
       <c r="AB255" s="2"/>
       <c r="AC255" s="2"/>
     </row>
-    <row r="256" spans="1:29" ht="23.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="256" spans="1:29" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A256" s="2">
         <v>255</v>
       </c>
@@ -21031,7 +21030,7 @@
       <c r="AB256" s="2"/>
       <c r="AC256" s="2"/>
     </row>
-    <row r="257" spans="1:29" ht="23.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="257" spans="1:29" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A257" s="2">
         <v>256</v>
       </c>
@@ -21092,7 +21091,7 @@
       <c r="AB257" s="2"/>
       <c r="AC257" s="2"/>
     </row>
-    <row r="258" spans="1:29" ht="23.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="258" spans="1:29" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A258" s="2">
         <v>257</v>
       </c>
@@ -21153,7 +21152,7 @@
       <c r="AB258" s="2"/>
       <c r="AC258" s="2"/>
     </row>
-    <row r="259" spans="1:29" ht="23.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="259" spans="1:29" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A259" s="2">
         <v>258</v>
       </c>
@@ -21214,7 +21213,7 @@
       <c r="AB259" s="2"/>
       <c r="AC259" s="2"/>
     </row>
-    <row r="260" spans="1:29" ht="23.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="260" spans="1:29" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A260" s="2">
         <v>259</v>
       </c>
@@ -21275,7 +21274,7 @@
       <c r="AB260" s="2"/>
       <c r="AC260" s="2"/>
     </row>
-    <row r="261" spans="1:29" ht="23.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="261" spans="1:29" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A261" s="2">
         <v>260</v>
       </c>
@@ -21336,7 +21335,7 @@
       <c r="AB261" s="2"/>
       <c r="AC261" s="2"/>
     </row>
-    <row r="262" spans="1:29" ht="23.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="262" spans="1:29" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A262" s="2">
         <v>261</v>
       </c>
@@ -21397,7 +21396,7 @@
       <c r="AB262" s="2"/>
       <c r="AC262" s="2"/>
     </row>
-    <row r="263" spans="1:29" ht="23.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="263" spans="1:29" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A263" s="2">
         <v>262</v>
       </c>
@@ -21458,7 +21457,7 @@
       <c r="AB263" s="2"/>
       <c r="AC263" s="2"/>
     </row>
-    <row r="264" spans="1:29" ht="23.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="264" spans="1:29" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A264" s="2">
         <v>263</v>
       </c>
@@ -21519,7 +21518,7 @@
       <c r="AB264" s="2"/>
       <c r="AC264" s="2"/>
     </row>
-    <row r="265" spans="1:29" ht="23.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="265" spans="1:29" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A265" s="2">
         <v>264</v>
       </c>
@@ -21641,7 +21640,7 @@
       <c r="AB266" s="2"/>
       <c r="AC266" s="2"/>
     </row>
-    <row r="267" spans="1:29" ht="23.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="267" spans="1:29" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A267" s="2">
         <v>266</v>
       </c>
@@ -21702,7 +21701,7 @@
       <c r="AB267" s="2"/>
       <c r="AC267" s="2"/>
     </row>
-    <row r="268" spans="1:29" ht="23.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="268" spans="1:29" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A268" s="2">
         <v>267</v>
       </c>
@@ -21763,7 +21762,7 @@
       <c r="AB268" s="2"/>
       <c r="AC268" s="2"/>
     </row>
-    <row r="269" spans="1:29" ht="23.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="269" spans="1:29" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A269" s="2">
         <v>268</v>
       </c>
@@ -21824,7 +21823,7 @@
       <c r="AB269" s="2"/>
       <c r="AC269" s="2"/>
     </row>
-    <row r="270" spans="1:29" ht="23.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="270" spans="1:29" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A270" s="2">
         <v>269</v>
       </c>
@@ -21885,7 +21884,7 @@
       <c r="AB270" s="2"/>
       <c r="AC270" s="2"/>
     </row>
-    <row r="271" spans="1:29" ht="23.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="271" spans="1:29" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A271" s="2">
         <v>270</v>
       </c>
@@ -21946,7 +21945,7 @@
       <c r="AB271" s="2"/>
       <c r="AC271" s="2"/>
     </row>
-    <row r="272" spans="1:29" ht="23.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="272" spans="1:29" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A272" s="2">
         <v>271</v>
       </c>
@@ -22007,7 +22006,7 @@
       <c r="AB272" s="2"/>
       <c r="AC272" s="2"/>
     </row>
-    <row r="273" spans="1:29" ht="23.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="273" spans="1:29" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A273" s="2">
         <v>272</v>
       </c>
@@ -22068,7 +22067,7 @@
       <c r="AB273" s="2"/>
       <c r="AC273" s="2"/>
     </row>
-    <row r="274" spans="1:29" ht="23.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="274" spans="1:29" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A274" s="2">
         <v>273</v>
       </c>
@@ -22129,7 +22128,7 @@
       <c r="AB274" s="2"/>
       <c r="AC274" s="2"/>
     </row>
-    <row r="275" spans="1:29" ht="23.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="275" spans="1:29" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A275" s="2">
         <v>274</v>
       </c>
@@ -22190,7 +22189,7 @@
       <c r="AB275" s="2"/>
       <c r="AC275" s="2"/>
     </row>
-    <row r="276" spans="1:29" ht="23.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="276" spans="1:29" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A276" s="2">
         <v>275</v>
       </c>
@@ -22251,7 +22250,7 @@
       <c r="AB276" s="2"/>
       <c r="AC276" s="2"/>
     </row>
-    <row r="277" spans="1:29" ht="23.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="277" spans="1:29" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A277" s="2">
         <v>276</v>
       </c>
@@ -22312,7 +22311,7 @@
       <c r="AB277" s="2"/>
       <c r="AC277" s="2"/>
     </row>
-    <row r="278" spans="1:29" ht="23.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="278" spans="1:29" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A278" s="2">
         <v>277</v>
       </c>
@@ -22373,7 +22372,7 @@
       <c r="AB278" s="2"/>
       <c r="AC278" s="2"/>
     </row>
-    <row r="279" spans="1:29" ht="23.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="279" spans="1:29" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A279" s="2">
         <v>278</v>
       </c>
@@ -22434,7 +22433,7 @@
       <c r="AB279" s="2"/>
       <c r="AC279" s="2"/>
     </row>
-    <row r="280" spans="1:29" ht="23.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="280" spans="1:29" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A280" s="2">
         <v>279</v>
       </c>
@@ -22495,7 +22494,7 @@
       <c r="AB280" s="2"/>
       <c r="AC280" s="2"/>
     </row>
-    <row r="281" spans="1:29" ht="23.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="281" spans="1:29" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A281" s="2">
         <v>280</v>
       </c>
@@ -22556,7 +22555,7 @@
       <c r="AB281" s="2"/>
       <c r="AC281" s="2"/>
     </row>
-    <row r="282" spans="1:29" ht="23.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="282" spans="1:29" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A282" s="2">
         <v>281</v>
       </c>
@@ -22617,7 +22616,7 @@
       <c r="AB282" s="2"/>
       <c r="AC282" s="2"/>
     </row>
-    <row r="283" spans="1:29" ht="23.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="283" spans="1:29" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A283" s="2">
         <v>282</v>
       </c>
@@ -22678,7 +22677,7 @@
       <c r="AB283" s="2"/>
       <c r="AC283" s="2"/>
     </row>
-    <row r="284" spans="1:29" ht="23.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="284" spans="1:29" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A284" s="2">
         <v>283</v>
       </c>
@@ -22739,7 +22738,7 @@
       <c r="AB284" s="2"/>
       <c r="AC284" s="2"/>
     </row>
-    <row r="285" spans="1:29" ht="23.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="285" spans="1:29" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A285" s="2">
         <v>284</v>
       </c>
@@ -22800,7 +22799,7 @@
       <c r="AB285" s="2"/>
       <c r="AC285" s="2"/>
     </row>
-    <row r="286" spans="1:29" ht="23.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="286" spans="1:29" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A286" s="2">
         <v>285</v>
       </c>
@@ -22861,7 +22860,7 @@
       <c r="AB286" s="2"/>
       <c r="AC286" s="2"/>
     </row>
-    <row r="287" spans="1:29" ht="23.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="287" spans="1:29" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A287" s="2">
         <v>286</v>
       </c>
@@ -22922,7 +22921,7 @@
       <c r="AB287" s="2"/>
       <c r="AC287" s="2"/>
     </row>
-    <row r="288" spans="1:29" ht="23.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="288" spans="1:29" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A288" s="2">
         <v>287</v>
       </c>
@@ -22983,7 +22982,7 @@
       <c r="AB288" s="2"/>
       <c r="AC288" s="2"/>
     </row>
-    <row r="289" spans="1:29" ht="23.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="289" spans="1:29" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A289" s="2">
         <v>288</v>
       </c>
@@ -23044,7 +23043,7 @@
       <c r="AB289" s="2"/>
       <c r="AC289" s="2"/>
     </row>
-    <row r="290" spans="1:29" ht="23.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="290" spans="1:29" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A290" s="2">
         <v>289</v>
       </c>
@@ -23105,7 +23104,7 @@
       <c r="AB290" s="2"/>
       <c r="AC290" s="2"/>
     </row>
-    <row r="291" spans="1:29" ht="23.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="291" spans="1:29" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A291" s="2">
         <v>290</v>
       </c>
@@ -23166,7 +23165,7 @@
       <c r="AB291" s="2"/>
       <c r="AC291" s="2"/>
     </row>
-    <row r="292" spans="1:29" ht="23.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="292" spans="1:29" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A292" s="2">
         <v>291</v>
       </c>
@@ -23227,7 +23226,7 @@
       <c r="AB292" s="2"/>
       <c r="AC292" s="2"/>
     </row>
-    <row r="293" spans="1:29" ht="23.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="293" spans="1:29" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A293" s="2">
         <v>292</v>
       </c>
@@ -23288,7 +23287,7 @@
       <c r="AB293" s="2"/>
       <c r="AC293" s="2"/>
     </row>
-    <row r="294" spans="1:29" ht="23.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="294" spans="1:29" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A294" s="2">
         <v>293</v>
       </c>
@@ -23349,7 +23348,7 @@
       <c r="AB294" s="2"/>
       <c r="AC294" s="2"/>
     </row>
-    <row r="295" spans="1:29" ht="23.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="295" spans="1:29" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A295" s="2">
         <v>294</v>
       </c>
@@ -23408,7 +23407,7 @@
       <c r="AB295" s="2"/>
       <c r="AC295" s="2"/>
     </row>
-    <row r="296" spans="1:29" ht="23.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="296" spans="1:29" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A296" s="2">
         <v>295</v>
       </c>
@@ -23469,7 +23468,7 @@
       <c r="AB296" s="2"/>
       <c r="AC296" s="2"/>
     </row>
-    <row r="297" spans="1:29" ht="23.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="297" spans="1:29" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A297" s="2">
         <v>296</v>
       </c>
@@ -23530,7 +23529,7 @@
       <c r="AB297" s="2"/>
       <c r="AC297" s="2"/>
     </row>
-    <row r="298" spans="1:29" ht="23.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="298" spans="1:29" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A298" s="2">
         <v>297</v>
       </c>
@@ -23591,7 +23590,7 @@
       <c r="AB298" s="2"/>
       <c r="AC298" s="2"/>
     </row>
-    <row r="299" spans="1:29" ht="23.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="299" spans="1:29" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A299" s="2">
         <v>298</v>
       </c>
@@ -23652,7 +23651,7 @@
       <c r="AB299" s="2"/>
       <c r="AC299" s="2"/>
     </row>
-    <row r="300" spans="1:29" ht="23.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="300" spans="1:29" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A300" s="2">
         <v>299</v>
       </c>
@@ -23713,7 +23712,7 @@
       <c r="AB300" s="2"/>
       <c r="AC300" s="2"/>
     </row>
-    <row r="301" spans="1:29" ht="23.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="301" spans="1:29" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A301" s="2">
         <v>300</v>
       </c>
@@ -23774,7 +23773,7 @@
       <c r="AB301" s="2"/>
       <c r="AC301" s="2"/>
     </row>
-    <row r="302" spans="1:29" ht="23.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="302" spans="1:29" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A302" s="2">
         <v>301</v>
       </c>
@@ -23835,7 +23834,7 @@
       <c r="AB302" s="2"/>
       <c r="AC302" s="2"/>
     </row>
-    <row r="303" spans="1:29" ht="23.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="303" spans="1:29" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A303" s="2">
         <v>302</v>
       </c>
@@ -23896,7 +23895,7 @@
       <c r="AB303" s="2"/>
       <c r="AC303" s="2"/>
     </row>
-    <row r="304" spans="1:29" ht="23.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="304" spans="1:29" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A304" s="2">
         <v>303</v>
       </c>
@@ -23957,7 +23956,7 @@
       <c r="AB304" s="2"/>
       <c r="AC304" s="2"/>
     </row>
-    <row r="305" spans="1:29" ht="23.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="305" spans="1:29" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A305" s="2">
         <v>304</v>
       </c>
@@ -24018,7 +24017,7 @@
       <c r="AB305" s="2"/>
       <c r="AC305" s="2"/>
     </row>
-    <row r="306" spans="1:29" ht="23.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="306" spans="1:29" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A306" s="2">
         <v>305</v>
       </c>
@@ -24079,7 +24078,7 @@
       <c r="AB306" s="2"/>
       <c r="AC306" s="2"/>
     </row>
-    <row r="307" spans="1:29" ht="23.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="307" spans="1:29" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A307" s="2">
         <v>306</v>
       </c>
@@ -24140,7 +24139,7 @@
       <c r="AB307" s="2"/>
       <c r="AC307" s="2"/>
     </row>
-    <row r="308" spans="1:29" ht="23.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="308" spans="1:29" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A308" s="2">
         <v>307</v>
       </c>
@@ -24201,7 +24200,7 @@
       <c r="AB308" s="2"/>
       <c r="AC308" s="2"/>
     </row>
-    <row r="309" spans="1:29" ht="23.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="309" spans="1:29" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A309" s="2">
         <v>308</v>
       </c>
@@ -24262,7 +24261,7 @@
       <c r="AB309" s="2"/>
       <c r="AC309" s="2"/>
     </row>
-    <row r="310" spans="1:29" ht="23.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="310" spans="1:29" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A310" s="2">
         <v>309</v>
       </c>
@@ -24323,7 +24322,7 @@
       <c r="AB310" s="2"/>
       <c r="AC310" s="2"/>
     </row>
-    <row r="311" spans="1:29" ht="23.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="311" spans="1:29" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A311" s="2">
         <v>310</v>
       </c>
@@ -24384,7 +24383,7 @@
       <c r="AB311" s="2"/>
       <c r="AC311" s="2"/>
     </row>
-    <row r="312" spans="1:29" ht="23.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="312" spans="1:29" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A312" s="2">
         <v>311</v>
       </c>
@@ -24445,7 +24444,7 @@
       <c r="AB312" s="2"/>
       <c r="AC312" s="2"/>
     </row>
-    <row r="313" spans="1:29" ht="23.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="313" spans="1:29" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A313" s="2">
         <v>312</v>
       </c>
@@ -24506,7 +24505,7 @@
       <c r="AB313" s="2"/>
       <c r="AC313" s="2"/>
     </row>
-    <row r="314" spans="1:29" ht="23.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="314" spans="1:29" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A314" s="2">
         <v>313</v>
       </c>
@@ -24567,7 +24566,7 @@
       <c r="AB314" s="2"/>
       <c r="AC314" s="2"/>
     </row>
-    <row r="315" spans="1:29" ht="23.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="315" spans="1:29" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A315" s="2">
         <v>314</v>
       </c>
@@ -24628,7 +24627,7 @@
       <c r="AB315" s="2"/>
       <c r="AC315" s="2"/>
     </row>
-    <row r="316" spans="1:29" ht="23.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="316" spans="1:29" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A316" s="2">
         <v>315</v>
       </c>
@@ -24689,7 +24688,7 @@
       <c r="AB316" s="2"/>
       <c r="AC316" s="2"/>
     </row>
-    <row r="317" spans="1:29" ht="23.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="317" spans="1:29" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A317" s="2">
         <v>316</v>
       </c>
@@ -24750,7 +24749,7 @@
       <c r="AB317" s="2"/>
       <c r="AC317" s="2"/>
     </row>
-    <row r="318" spans="1:29" ht="23.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="318" spans="1:29" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A318" s="2">
         <v>317</v>
       </c>
@@ -24811,7 +24810,7 @@
       <c r="AB318" s="2"/>
       <c r="AC318" s="2"/>
     </row>
-    <row r="319" spans="1:29" ht="23.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="319" spans="1:29" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A319" s="2">
         <v>318</v>
       </c>
@@ -24872,7 +24871,7 @@
       <c r="AB319" s="2"/>
       <c r="AC319" s="2"/>
     </row>
-    <row r="320" spans="1:29" ht="23.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="320" spans="1:29" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A320" s="2">
         <v>319</v>
       </c>
@@ -24933,7 +24932,7 @@
       <c r="AB320" s="2"/>
       <c r="AC320" s="2"/>
     </row>
-    <row r="321" spans="1:29" ht="23.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="321" spans="1:29" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A321" s="2">
         <v>320</v>
       </c>
@@ -24994,7 +24993,7 @@
       <c r="AB321" s="2"/>
       <c r="AC321" s="2"/>
     </row>
-    <row r="322" spans="1:29" ht="23.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="322" spans="1:29" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A322" s="2">
         <v>321</v>
       </c>
@@ -25055,7 +25054,7 @@
       <c r="AB322" s="2"/>
       <c r="AC322" s="2"/>
     </row>
-    <row r="323" spans="1:29" ht="23.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="323" spans="1:29" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A323" s="2">
         <v>322</v>
       </c>
@@ -25116,7 +25115,7 @@
       <c r="AB323" s="2"/>
       <c r="AC323" s="2"/>
     </row>
-    <row r="324" spans="1:29" ht="23.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="324" spans="1:29" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A324" s="2">
         <v>323</v>
       </c>
@@ -25177,7 +25176,7 @@
       <c r="AB324" s="2"/>
       <c r="AC324" s="2"/>
     </row>
-    <row r="325" spans="1:29" ht="23.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="325" spans="1:29" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A325" s="2">
         <v>324</v>
       </c>
@@ -25238,7 +25237,7 @@
       <c r="AB325" s="2"/>
       <c r="AC325" s="2"/>
     </row>
-    <row r="326" spans="1:29" ht="23.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="326" spans="1:29" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A326" s="2">
         <v>325</v>
       </c>
@@ -25299,7 +25298,7 @@
       <c r="AB326" s="2"/>
       <c r="AC326" s="2"/>
     </row>
-    <row r="327" spans="1:29" ht="23.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="327" spans="1:29" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A327" s="2">
         <v>326</v>
       </c>
@@ -25360,7 +25359,7 @@
       <c r="AB327" s="2"/>
       <c r="AC327" s="2"/>
     </row>
-    <row r="328" spans="1:29" ht="23.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="328" spans="1:29" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A328" s="2">
         <v>327</v>
       </c>
@@ -25421,7 +25420,7 @@
       <c r="AB328" s="2"/>
       <c r="AC328" s="2"/>
     </row>
-    <row r="329" spans="1:29" ht="23.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="329" spans="1:29" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A329" s="2">
         <v>328</v>
       </c>
@@ -25482,7 +25481,7 @@
       <c r="AB329" s="2"/>
       <c r="AC329" s="2"/>
     </row>
-    <row r="330" spans="1:29" ht="23.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="330" spans="1:29" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A330" s="2">
         <v>329</v>
       </c>
@@ -25543,7 +25542,7 @@
       <c r="AB330" s="2"/>
       <c r="AC330" s="2"/>
     </row>
-    <row r="331" spans="1:29" ht="23.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="331" spans="1:29" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A331" s="2">
         <v>330</v>
       </c>
@@ -25604,7 +25603,7 @@
       <c r="AB331" s="2"/>
       <c r="AC331" s="2"/>
     </row>
-    <row r="332" spans="1:29" ht="23.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="332" spans="1:29" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A332" s="2">
         <v>331</v>
       </c>
@@ -25665,7 +25664,7 @@
       <c r="AB332" s="2"/>
       <c r="AC332" s="2"/>
     </row>
-    <row r="333" spans="1:29" ht="23.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="333" spans="1:29" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A333" s="2">
         <v>332</v>
       </c>
@@ -25726,7 +25725,7 @@
       <c r="AB333" s="2"/>
       <c r="AC333" s="2"/>
     </row>
-    <row r="334" spans="1:29" ht="23.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="334" spans="1:29" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A334" s="2">
         <v>333</v>
       </c>
@@ -25787,7 +25786,7 @@
       <c r="AB334" s="2"/>
       <c r="AC334" s="2"/>
     </row>
-    <row r="335" spans="1:29" ht="23.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="335" spans="1:29" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A335" s="2">
         <v>334</v>
       </c>
@@ -25848,7 +25847,7 @@
       <c r="AB335" s="2"/>
       <c r="AC335" s="2"/>
     </row>
-    <row r="336" spans="1:29" ht="23.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="336" spans="1:29" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A336" s="2">
         <v>335</v>
       </c>
@@ -25909,7 +25908,7 @@
       <c r="AB336" s="2"/>
       <c r="AC336" s="2"/>
     </row>
-    <row r="337" spans="1:29" ht="23.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="337" spans="1:29" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A337" s="2">
         <v>336</v>
       </c>
@@ -25970,7 +25969,7 @@
       <c r="AB337" s="2"/>
       <c r="AC337" s="2"/>
     </row>
-    <row r="338" spans="1:29" ht="23.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="338" spans="1:29" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A338" s="2">
         <v>337</v>
       </c>
@@ -26031,7 +26030,7 @@
       <c r="AB338" s="2"/>
       <c r="AC338" s="2"/>
     </row>
-    <row r="339" spans="1:29" ht="23.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="339" spans="1:29" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A339" s="2">
         <v>338</v>
       </c>
@@ -26092,7 +26091,7 @@
       <c r="AB339" s="2"/>
       <c r="AC339" s="2"/>
     </row>
-    <row r="340" spans="1:29" ht="23.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="340" spans="1:29" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A340" s="2">
         <v>339</v>
       </c>
@@ -26153,7 +26152,7 @@
       <c r="AB340" s="2"/>
       <c r="AC340" s="2"/>
     </row>
-    <row r="341" spans="1:29" ht="23.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="341" spans="1:29" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A341" s="2">
         <v>340</v>
       </c>
@@ -26214,7 +26213,7 @@
       <c r="AB341" s="2"/>
       <c r="AC341" s="2"/>
     </row>
-    <row r="342" spans="1:29" ht="23.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="342" spans="1:29" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A342" s="2">
         <v>341</v>
       </c>
@@ -26275,7 +26274,7 @@
       <c r="AB342" s="2"/>
       <c r="AC342" s="2"/>
     </row>
-    <row r="343" spans="1:29" ht="23.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="343" spans="1:29" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A343" s="2">
         <v>342</v>
       </c>
@@ -26336,7 +26335,7 @@
       <c r="AB343" s="2"/>
       <c r="AC343" s="2"/>
     </row>
-    <row r="344" spans="1:29" ht="23.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="344" spans="1:29" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A344" s="2">
         <v>343</v>
       </c>
@@ -26397,7 +26396,7 @@
       <c r="AB344" s="2"/>
       <c r="AC344" s="2"/>
     </row>
-    <row r="345" spans="1:29" ht="23.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="345" spans="1:29" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A345" s="2">
         <v>344</v>
       </c>
@@ -26458,7 +26457,7 @@
       <c r="AB345" s="2"/>
       <c r="AC345" s="2"/>
     </row>
-    <row r="346" spans="1:29" ht="23.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="346" spans="1:29" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A346" s="2">
         <v>345</v>
       </c>
@@ -26519,7 +26518,7 @@
       <c r="AB346" s="2"/>
       <c r="AC346" s="2"/>
     </row>
-    <row r="347" spans="1:29" ht="23.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="347" spans="1:29" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A347" s="2">
         <v>346</v>
       </c>
@@ -26580,7 +26579,7 @@
       <c r="AB347" s="2"/>
       <c r="AC347" s="2"/>
     </row>
-    <row r="348" spans="1:29" ht="23.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="348" spans="1:29" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A348" s="2">
         <v>347</v>
       </c>
@@ -26641,7 +26640,7 @@
       <c r="AB348" s="2"/>
       <c r="AC348" s="2"/>
     </row>
-    <row r="349" spans="1:29" ht="23.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="349" spans="1:29" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A349" s="2">
         <v>348</v>
       </c>
@@ -26702,7 +26701,7 @@
       <c r="AB349" s="2"/>
       <c r="AC349" s="2"/>
     </row>
-    <row r="350" spans="1:29" ht="23.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="350" spans="1:29" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A350" s="2">
         <v>349</v>
       </c>
@@ -26763,7 +26762,7 @@
       <c r="AB350" s="2"/>
       <c r="AC350" s="2"/>
     </row>
-    <row r="351" spans="1:29" ht="23.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="351" spans="1:29" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A351" s="2">
         <v>350</v>
       </c>
@@ -26824,7 +26823,7 @@
       <c r="AB351" s="2"/>
       <c r="AC351" s="2"/>
     </row>
-    <row r="352" spans="1:29" ht="23.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="352" spans="1:29" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A352" s="2">
         <v>351</v>
       </c>
@@ -26885,7 +26884,7 @@
       <c r="AB352" s="2"/>
       <c r="AC352" s="2"/>
     </row>
-    <row r="353" spans="1:29" ht="23.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="353" spans="1:29" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A353" s="2">
         <v>352</v>
       </c>
@@ -26946,7 +26945,7 @@
       <c r="AB353" s="2"/>
       <c r="AC353" s="2"/>
     </row>
-    <row r="354" spans="1:29" ht="23.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="354" spans="1:29" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A354" s="2">
         <v>353</v>
       </c>
@@ -27007,7 +27006,7 @@
       <c r="AB354" s="2"/>
       <c r="AC354" s="2"/>
     </row>
-    <row r="355" spans="1:29" ht="23.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="355" spans="1:29" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A355" s="2">
         <v>354</v>
       </c>
@@ -27068,7 +27067,7 @@
       <c r="AB355" s="2"/>
       <c r="AC355" s="2"/>
     </row>
-    <row r="356" spans="1:29" ht="23.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="356" spans="1:29" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A356" s="2">
         <v>355</v>
       </c>
@@ -27129,7 +27128,7 @@
       <c r="AB356" s="2"/>
       <c r="AC356" s="2"/>
     </row>
-    <row r="357" spans="1:29" ht="23.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="357" spans="1:29" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A357" s="2">
         <v>356</v>
       </c>
@@ -27190,7 +27189,7 @@
       <c r="AB357" s="2"/>
       <c r="AC357" s="2"/>
     </row>
-    <row r="358" spans="1:29" ht="23.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="358" spans="1:29" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A358" s="2">
         <v>357</v>
       </c>
@@ -27251,7 +27250,7 @@
       <c r="AB358" s="2"/>
       <c r="AC358" s="2"/>
     </row>
-    <row r="359" spans="1:29" ht="23.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="359" spans="1:29" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A359" s="2">
         <v>358</v>
       </c>
@@ -27312,7 +27311,7 @@
       <c r="AB359" s="2"/>
       <c r="AC359" s="2"/>
     </row>
-    <row r="360" spans="1:29" ht="23.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="360" spans="1:29" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A360" s="2">
         <v>359</v>
       </c>
@@ -27373,7 +27372,7 @@
       <c r="AB360" s="2"/>
       <c r="AC360" s="2"/>
     </row>
-    <row r="361" spans="1:29" ht="23.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="361" spans="1:29" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A361" s="2">
         <v>360</v>
       </c>
@@ -27434,7 +27433,7 @@
       <c r="AB361" s="2"/>
       <c r="AC361" s="2"/>
     </row>
-    <row r="362" spans="1:29" ht="23.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="362" spans="1:29" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A362" s="2">
         <v>361</v>
       </c>
@@ -27495,7 +27494,7 @@
       <c r="AB362" s="2"/>
       <c r="AC362" s="2"/>
     </row>
-    <row r="363" spans="1:29" ht="23.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="363" spans="1:29" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A363" s="2">
         <v>362</v>
       </c>
@@ -27556,7 +27555,7 @@
       <c r="AB363" s="2"/>
       <c r="AC363" s="2"/>
     </row>
-    <row r="364" spans="1:29" ht="23.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="364" spans="1:29" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A364" s="2">
         <v>363</v>
       </c>
@@ -27617,7 +27616,7 @@
       <c r="AB364" s="2"/>
       <c r="AC364" s="2"/>
     </row>
-    <row r="365" spans="1:29" ht="23.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="365" spans="1:29" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A365" s="2">
         <v>364</v>
       </c>
@@ -27678,7 +27677,7 @@
       <c r="AB365" s="2"/>
       <c r="AC365" s="2"/>
     </row>
-    <row r="366" spans="1:29" ht="23.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="366" spans="1:29" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A366" s="2">
         <v>365</v>
       </c>
@@ -27739,7 +27738,7 @@
       <c r="AB366" s="2"/>
       <c r="AC366" s="2"/>
     </row>
-    <row r="367" spans="1:29" ht="23.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="367" spans="1:29" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A367" s="2">
         <v>366</v>
       </c>
@@ -27800,7 +27799,7 @@
       <c r="AB367" s="2"/>
       <c r="AC367" s="2"/>
     </row>
-    <row r="368" spans="1:29" ht="23.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="368" spans="1:29" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A368" s="2">
         <v>367</v>
       </c>
@@ -27861,7 +27860,7 @@
       <c r="AB368" s="2"/>
       <c r="AC368" s="2"/>
     </row>
-    <row r="369" spans="1:29" ht="23.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="369" spans="1:29" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A369" s="2">
         <v>368</v>
       </c>
@@ -27922,7 +27921,7 @@
       <c r="AB369" s="2"/>
       <c r="AC369" s="2"/>
     </row>
-    <row r="370" spans="1:29" ht="23.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="370" spans="1:29" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A370" s="2">
         <v>369</v>
       </c>
@@ -27983,7 +27982,7 @@
       <c r="AB370" s="2"/>
       <c r="AC370" s="2"/>
     </row>
-    <row r="371" spans="1:29" ht="23.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="371" spans="1:29" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A371" s="2">
         <v>370</v>
       </c>
@@ -28044,7 +28043,7 @@
       <c r="AB371" s="2"/>
       <c r="AC371" s="2"/>
     </row>
-    <row r="372" spans="1:29" ht="23.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="372" spans="1:29" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A372" s="2">
         <v>371</v>
       </c>
@@ -28105,7 +28104,7 @@
       <c r="AB372" s="2"/>
       <c r="AC372" s="2"/>
     </row>
-    <row r="373" spans="1:29" ht="23.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="373" spans="1:29" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A373" s="2">
         <v>372</v>
       </c>
@@ -28166,7 +28165,7 @@
       <c r="AB373" s="2"/>
       <c r="AC373" s="2"/>
     </row>
-    <row r="374" spans="1:29" ht="23.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="374" spans="1:29" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A374" s="2">
         <v>373</v>
       </c>
@@ -28227,7 +28226,7 @@
       <c r="AB374" s="2"/>
       <c r="AC374" s="2"/>
     </row>
-    <row r="375" spans="1:29" ht="23.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="375" spans="1:29" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A375" s="2">
         <v>374</v>
       </c>
@@ -28288,7 +28287,7 @@
       <c r="AB375" s="2"/>
       <c r="AC375" s="2"/>
     </row>
-    <row r="376" spans="1:29" ht="23.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="376" spans="1:29" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A376" s="2">
         <v>375</v>
       </c>
@@ -28349,7 +28348,7 @@
       <c r="AB376" s="2"/>
       <c r="AC376" s="2"/>
     </row>
-    <row r="377" spans="1:29" ht="23.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="377" spans="1:29" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A377" s="2">
         <v>376</v>
       </c>
@@ -28410,7 +28409,7 @@
       <c r="AB377" s="2"/>
       <c r="AC377" s="2"/>
     </row>
-    <row r="378" spans="1:29" ht="23.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="378" spans="1:29" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A378" s="2">
         <v>377</v>
       </c>
@@ -28471,7 +28470,7 @@
       <c r="AB378" s="2"/>
       <c r="AC378" s="2"/>
     </row>
-    <row r="379" spans="1:29" ht="23.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="379" spans="1:29" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A379" s="2">
         <v>378</v>
       </c>
@@ -28532,7 +28531,7 @@
       <c r="AB379" s="2"/>
       <c r="AC379" s="2"/>
     </row>
-    <row r="380" spans="1:29" ht="23.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="380" spans="1:29" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A380" s="2">
         <v>379</v>
       </c>
@@ -28593,7 +28592,7 @@
       <c r="AB380" s="2"/>
       <c r="AC380" s="2"/>
     </row>
-    <row r="381" spans="1:29" ht="23.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="381" spans="1:29" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A381" s="2">
         <v>380</v>
       </c>
@@ -28654,7 +28653,7 @@
       <c r="AB381" s="2"/>
       <c r="AC381" s="2"/>
     </row>
-    <row r="382" spans="1:29" ht="23.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="382" spans="1:29" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A382" s="2">
         <v>381</v>
       </c>
@@ -28715,7 +28714,7 @@
       <c r="AB382" s="2"/>
       <c r="AC382" s="2"/>
     </row>
-    <row r="383" spans="1:29" ht="23.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="383" spans="1:29" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A383" s="2">
         <v>382</v>
       </c>
@@ -28776,7 +28775,7 @@
       <c r="AB383" s="2"/>
       <c r="AC383" s="2"/>
     </row>
-    <row r="384" spans="1:29" ht="23.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="384" spans="1:29" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A384" s="2">
         <v>383</v>
       </c>
@@ -28837,7 +28836,7 @@
       <c r="AB384" s="2"/>
       <c r="AC384" s="2"/>
     </row>
-    <row r="385" spans="1:29" ht="23.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="385" spans="1:29" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A385" s="2">
         <v>384</v>
       </c>
@@ -28898,7 +28897,7 @@
       <c r="AB385" s="2"/>
       <c r="AC385" s="2"/>
     </row>
-    <row r="386" spans="1:29" ht="23.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="386" spans="1:29" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A386" s="2">
         <v>385</v>
       </c>
@@ -28959,7 +28958,7 @@
       <c r="AB386" s="2"/>
       <c r="AC386" s="2"/>
     </row>
-    <row r="387" spans="1:29" ht="23.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="387" spans="1:29" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A387" s="2">
         <v>386</v>
       </c>
@@ -29020,7 +29019,7 @@
       <c r="AB387" s="2"/>
       <c r="AC387" s="2"/>
     </row>
-    <row r="388" spans="1:29" ht="23.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="388" spans="1:29" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A388" s="2">
         <v>387</v>
       </c>
@@ -29081,7 +29080,7 @@
       <c r="AB388" s="2"/>
       <c r="AC388" s="2"/>
     </row>
-    <row r="389" spans="1:29" ht="23.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="389" spans="1:29" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A389" s="2">
         <v>388</v>
       </c>
@@ -29143,13 +29142,6 @@
       <c r="AC389" s="2"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:R389" xr:uid="{90D3818D-47CE-41E6-8913-CED8EE4E3F8A}">
-    <filterColumn colId="17">
-      <filters>
-        <filter val="E"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>